<commit_message>
Adicionando Authorization Server na Aplicação
</commit_message>
<xml_diff>
--- a/src/main/resources/docs/especialista-spring-rest.xlsx
+++ b/src/main/resources/docs/especialista-spring-rest.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="467">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="471">
   <si>
     <t xml:space="preserve">TERMOS</t>
   </si>
@@ -2917,6 +2917,31 @@
       </rPr>
       <t xml:space="preserve">)</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Autenticação por Banco de Dados</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Talvez seja necessário a criação de uma tablea para armazenar as aplicações que farão a solicitação de Token
+- Para isso setamos a configuração do Authorization Server para buscar os dados de acesso
+- Em ClientDetailsServiceConfigurer configuraremos os clients como jdbc
+- Para debugar possíveis erros utilizar:
+logging.level.org.springframework=DEBUG
+- Também é necessário a criação da tabela oauth_client_details</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tabela OAUTH_CLIENT_DETAILS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">client_id: id da aplicação
+client_secret: password encoded
+scope: READ,WRITE
+authorized_grant_types: password ou authorizathion_code
+web_server_redirect_uri: Endereço de redirecionamento ou null
+access_token_validity: 60 * 60 * 6 (validade de 6 horas)
+refresh_token_validity: 60 * 24 * 60 * 60 (2 meses)
+autoaprove: se ‘true’ aprova automaticamente as permissões
+Authorities: define authorities padrão para o toke ‘EDITAR_COZINHAS,EDITAR_RESTAURANTES’ </t>
   </si>
   <si>
     <t xml:space="preserve">ERRO</t>
@@ -3228,10 +3253,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:B235"/>
+  <dimension ref="A2:B237"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A232" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B235" activeCellId="0" sqref="B235"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A233" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F235" activeCellId="0" sqref="F235"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5101,6 +5126,22 @@
       </c>
       <c r="B235" s="1" t="s">
         <v>461</v>
+      </c>
+    </row>
+    <row r="236" customFormat="false" ht="69.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A236" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="B236" s="1" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="237" customFormat="false" ht="104.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A237" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="B237" s="1" t="s">
+        <v>465</v>
       </c>
     </row>
   </sheetData>
@@ -5133,7 +5174,7 @@
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="10" t="s">
-        <v>462</v>
+        <v>466</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>1</v>
@@ -5145,10 +5186,10 @@
         <v>400</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>463</v>
+        <v>467</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>464</v>
+        <v>468</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5156,10 +5197,10 @@
         <v>404</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>465</v>
+        <v>469</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>466</v>
+        <v>470</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
feat: adding oauth2 security in openApi
</commit_message>
<xml_diff>
--- a/src/main/resources/docs/especialista-spring-rest.xlsx
+++ b/src/main/resources/docs/especialista-spring-rest.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1043" uniqueCount="974">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1061" uniqueCount="988">
   <si>
     <t xml:space="preserve">Especialista Spring Rest</t>
   </si>
@@ -4468,10 +4468,96 @@
   <si>
     <t xml:space="preserve">Adicione as seguintes dependências ao projeto:
 Springdoc-openapi-ui, springdoc-openapi-hateoas e springdoc-openapi-security
-Todos na versao 1.6.9 com Spring na versão 2.7.1 e java 17</t>
+Todos na versao 1.6.9 com Spring na versão 2.7.1 e java 17
+Com isso é possível acessar a documentacao em swagger-ui/index.html</t>
   </si>
   <si>
     <t xml:space="preserve">26.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bean OpenApi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No Bean do OpenApi estão as configurações de inicialização do swagger
+Estão as configurações que podemos customizar:
+@Configuration
+public class SpringDocConfig {…}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Limitando presença de Controllers na Documentação</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Faz com que seja possível limitar quais os pacotes serão escaneados para apresentação da documentação
+Em application.properties insira a configuração:
+springdoc.packages-to-scan=com.algaworks.algafood.api
+Também podemos limitar a descoberta por paths:
+springdoc.path-to-match=/v1/**,/v2/**</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bean GroupedOpenApi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Utilizado para fazer separações na documentação entre versionamentos de controladores
+- Criamos um Bean para agrupar todos os controllers de uma versão:
+@Bean
+public GroupedOpenApi v1Api() {
+return GroupedOpenApi.builder()
+.group("v1")
+.pathsToMatch("/v1/**")
+.build();
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Segurança na Documentação
+Botão Authorize</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Para realizar autenticação na documentação para envio de requisições usamos a anotação @SecurityScheme
+@Configuration
+@SecurityScheme(name = "security_auth", type = SecuritySchemeType.OAUTH2)@Configuration
+@SecurityScheme(
+name = "security_auth",
+type = SecuritySchemeType.OAUTH2,
+flows =  @OAuthFlows(authorizationCode = @OAuthFlow(
+authorizationUrl = "${springdoc.oAuthFlow.authorizationUrl}",
+tokenUrl = "${springdoc.oAuthFlow.tokenUrl}",
+scopes = {
+@OAuthScope(name = "READ", description = "read scope"),
+@OAuthScope(name = "WRITE", description = "write scope"),
+}
+)))
+Public class SpringDocConfig {…}
+- Com isso um botão de Authorize aparecerá ao canto da tela para autenticar seu usuário para requisições
+- Crie as chaves no application.properties e configura a autenticação
+springdoc.oAuthFlow.authorizationUrl=http://localhost:9000/oauth/authorize
+springdoc.oAuthFlow.tokenUrl=http://localhost:9000/oauth/token</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Preparando Autorização</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Definir o client para preenchimento automático:
+springdoc.swagger-ui.oauth.client-id=algafood-web
+springdoc.swagger-ui.oauth.client-secret=web123
+E utilizaça o do PKCE:
+springdoc.swagger-ui.oauth.use-pkce-with-authorization-code-grant=true
+- Em oauth_client_details adicione o redirecionamento e permissões do usuário
+Na coluna ‘scope’ deve conter: 
+  'READ,WRITE', 'password,authorization_code', 'http://localhost:9000,http://localhost:9000/swagger-ui/oauth2-redirect.html', null,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adiciona no Controllers a Anotação de Segurança</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Para autorização do fluxo que implementamos é necessário adicionar uma anotação sobre os controladores com o nome da security que criamos
+@SecurityRequirement(name="security_auth")
+public interface CidadeControllerOpenApi {…}</t>
   </si>
   <si>
     <t xml:space="preserve">ERRO</t>
@@ -4833,8 +4919,8 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A359" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B364" activeCellId="0" sqref="B364"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A367" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B370" activeCellId="0" sqref="B370"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8724,7 +8810,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="363" customFormat="false" ht="40.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="363" customFormat="false" ht="61.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A363" s="6" t="s">
         <v>966</v>
       </c>
@@ -8735,35 +8821,71 @@
         <v>968</v>
       </c>
     </row>
-    <row r="364" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A364" s="6"/>
-      <c r="B364" s="6"/>
-      <c r="C364" s="6"/>
-    </row>
-    <row r="365" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A365" s="6"/>
-      <c r="B365" s="6"/>
-      <c r="C365" s="6"/>
-    </row>
-    <row r="366" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A366" s="6"/>
-      <c r="B366" s="6"/>
-      <c r="C366" s="6"/>
-    </row>
-    <row r="367" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A367" s="6"/>
-      <c r="B367" s="6"/>
-      <c r="C367" s="6"/>
-    </row>
-    <row r="368" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A368" s="6"/>
-      <c r="B368" s="6"/>
-      <c r="C368" s="6"/>
-    </row>
-    <row r="369" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A369" s="6"/>
-      <c r="B369" s="6"/>
-      <c r="C369" s="6"/>
+    <row r="364" customFormat="false" ht="69.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A364" s="6" t="s">
+        <v>969</v>
+      </c>
+      <c r="B364" s="6" t="s">
+        <v>970</v>
+      </c>
+      <c r="C364" s="6" t="s">
+        <v>968</v>
+      </c>
+    </row>
+    <row r="365" customFormat="false" ht="79.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A365" s="6" t="s">
+        <v>971</v>
+      </c>
+      <c r="B365" s="6" t="s">
+        <v>972</v>
+      </c>
+      <c r="C365" s="6" t="s">
+        <v>968</v>
+      </c>
+    </row>
+    <row r="366" customFormat="false" ht="121.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A366" s="6" t="s">
+        <v>973</v>
+      </c>
+      <c r="B366" s="6" t="s">
+        <v>974</v>
+      </c>
+      <c r="C366" s="6" t="s">
+        <v>975</v>
+      </c>
+    </row>
+    <row r="367" customFormat="false" ht="242.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A367" s="6" t="s">
+        <v>976</v>
+      </c>
+      <c r="B367" s="6" t="s">
+        <v>977</v>
+      </c>
+      <c r="C367" s="6" t="s">
+        <v>978</v>
+      </c>
+    </row>
+    <row r="368" customFormat="false" ht="131.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A368" s="6" t="s">
+        <v>979</v>
+      </c>
+      <c r="B368" s="6" t="s">
+        <v>980</v>
+      </c>
+      <c r="C368" s="6" t="s">
+        <v>978</v>
+      </c>
+    </row>
+    <row r="369" customFormat="false" ht="40.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A369" s="6" t="s">
+        <v>981</v>
+      </c>
+      <c r="B369" s="6" t="s">
+        <v>982</v>
+      </c>
+      <c r="C369" s="6" t="s">
+        <v>978</v>
+      </c>
     </row>
     <row r="370" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A370" s="6"/>
@@ -8860,16 +8982,8 @@
       <c r="B388" s="6"/>
       <c r="C388" s="6"/>
     </row>
-    <row r="389" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A389" s="6"/>
-      <c r="B389" s="6"/>
-      <c r="C389" s="6"/>
-    </row>
-    <row r="390" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A390" s="6"/>
-      <c r="B390" s="6"/>
-      <c r="C390" s="6"/>
-    </row>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="1">
@@ -8907,7 +9021,7 @@
   <sheetData>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="8" t="s">
-        <v>969</v>
+        <v>983</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>2</v>
@@ -8919,10 +9033,10 @@
         <v>400</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>970</v>
+        <v>984</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>971</v>
+        <v>985</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8930,10 +9044,10 @@
         <v>404</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>972</v>
+        <v>986</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>973</v>
+        <v>987</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
feat: adding openApi customization
</commit_message>
<xml_diff>
--- a/src/main/resources/docs/especialista-spring-rest.xlsx
+++ b/src/main/resources/docs/especialista-spring-rest.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1061" uniqueCount="988">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1087" uniqueCount="1013">
   <si>
     <t xml:space="preserve">Especialista Spring Rest</t>
   </si>
@@ -4558,6 +4558,109 @@
     <t xml:space="preserve">Para autorização do fluxo que implementamos é necessário adicionar uma anotação sobre os controladores com o nome da security que criamos
 @SecurityRequirement(name="security_auth")
 public interface CidadeControllerOpenApi {…}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Autorizando</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ao clicar no botão ao canto da tela em documentação é possível observar que tudo está preenchido e configurado
+Selecione todos os escopos e clique em autorizar
+Preencha com as credenciais de seu usuário joao.ger@algafood.com.br</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Criação de TAGs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Servem para agrupar alguns recursos semelhantes definindo nome e descrição
+@Tag(name = "Cidades", description = "Gerencia as Cidades")
+public interface CidadeControllerOpenApi {…}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26.6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Descrevendo Operações</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Descreve uma aoperação de um endpoint na documentação:
+	@Operation(summary = "Cadastra uma cidade", description = "Cadastro de uma cidade, necessita de um estado e um nome válido")
+	CidadeModel adicionar(CidadeInput cidadeInput);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26.7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Descrevendo Parâmetros</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Define os parâmetros nos recursos attravés da anotação @Parameter e também @Requestbody do swagger
+Também é possível definir um exemplo que autocompletará na documentação:
+CidadeModel buscar(@Parameter(description = "ID de uma cidade", example = "1", required = true) Long cidadeId);
+	CidadeModel adicionar(@RequestBody(description = "Representação de uma nova cidade", required = true) CidadeInput cidadeInput);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26.8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Descrevendo Modelos de Representação</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Podemos descrever os Modelos de Representação, seus campos e classes
+- Essa configuração é refletida tanto requisição quanto nos modelos representados abaixo na documentação
+@NotBlank
+@Schema(example = "Uberlândia")
+private String nome;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26.9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Descrevendo Validação de Modelo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Para definir as validações de modelo o springDocs consegue aproveitar as anotações já definidas como @NotBlank, @NotNull
+- Mas podemos definir na própria anotação caso necessário com required = true
+- Porém é preferível continuar utilizando as anotações do Javax
+@Schema(example = "Uberlândia", required = true)
+private String nome;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26.10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Definindo Códigos de Respostas 
+De Forma Global</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Necessário a criação de um Bean OpenAPICustomizer
+Essa customização faz um iteração sobre os paths da nossa aplicação e adiciona ApiResponse Globeis nele de acordo com seus status
+                        ApiResponse apiResponseNaoEncontrado = new ApiResponse().description("Recurso não encontrado");
+                        responses.addApiResponse("406", apiResponseNaoEncontrado);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26.11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Descrevendo StatusCode 
+Para Respostas Específicas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Na anotação de @Operation basta passar o código e descrição
+	@Operation(summary = "Busca uma cidade por Id", responses = {
+			@ApiResponse(responseCode = "200"),
+			@ApiResponse(responseCode = "400", description = "ID da cidade inválido",
+					content = @Content(schema = @Schema))})
+	CidadeModel buscar(@Parameter(description = "ID de uma cidade", example = "1", required = true) Long cidadeId);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26.12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Descrevendo StatusCode
+De Acordo com Método HTTP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26.13</t>
   </si>
   <si>
     <t xml:space="preserve">ERRO</t>
@@ -4919,8 +5022,8 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A367" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B370" activeCellId="0" sqref="B370"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A376" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C379" activeCellId="0" sqref="C379"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8865,7 +8968,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="368" customFormat="false" ht="131.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="368" customFormat="false" ht="121.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A368" s="6" t="s">
         <v>979</v>
       </c>
@@ -8887,50 +8990,102 @@
         <v>978</v>
       </c>
     </row>
-    <row r="370" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A370" s="6"/>
-      <c r="B370" s="6"/>
-      <c r="C370" s="6"/>
-    </row>
-    <row r="371" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A371" s="6"/>
-      <c r="B371" s="6"/>
-      <c r="C371" s="6"/>
-    </row>
-    <row r="372" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A372" s="6"/>
-      <c r="B372" s="6"/>
-      <c r="C372" s="6"/>
-    </row>
-    <row r="373" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A373" s="6"/>
-      <c r="B373" s="6"/>
-      <c r="C373" s="6"/>
-    </row>
-    <row r="374" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A374" s="6"/>
-      <c r="B374" s="6"/>
-      <c r="C374" s="6"/>
-    </row>
-    <row r="375" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A375" s="6"/>
-      <c r="B375" s="6"/>
-      <c r="C375" s="6"/>
-    </row>
-    <row r="376" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A376" s="6"/>
-      <c r="B376" s="6"/>
-      <c r="C376" s="6"/>
-    </row>
-    <row r="377" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A377" s="6"/>
-      <c r="B377" s="6"/>
-      <c r="C377" s="6"/>
+    <row r="370" customFormat="false" ht="41.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A370" s="6" t="s">
+        <v>983</v>
+      </c>
+      <c r="B370" s="6" t="s">
+        <v>984</v>
+      </c>
+      <c r="C370" s="6" t="s">
+        <v>978</v>
+      </c>
+    </row>
+    <row r="371" customFormat="false" ht="43.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A371" s="6" t="s">
+        <v>985</v>
+      </c>
+      <c r="B371" s="6" t="s">
+        <v>986</v>
+      </c>
+      <c r="C371" s="6" t="s">
+        <v>987</v>
+      </c>
+    </row>
+    <row r="372" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A372" s="6" t="s">
+        <v>988</v>
+      </c>
+      <c r="B372" s="6" t="s">
+        <v>989</v>
+      </c>
+      <c r="C372" s="6" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="373" customFormat="false" ht="70.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A373" s="6" t="s">
+        <v>991</v>
+      </c>
+      <c r="B373" s="6" t="s">
+        <v>992</v>
+      </c>
+      <c r="C373" s="6" t="s">
+        <v>993</v>
+      </c>
+    </row>
+    <row r="374" customFormat="false" ht="74.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A374" s="6" t="s">
+        <v>994</v>
+      </c>
+      <c r="B374" s="6" t="s">
+        <v>995</v>
+      </c>
+      <c r="C374" s="6" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="375" customFormat="false" ht="75.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A375" s="6" t="s">
+        <v>997</v>
+      </c>
+      <c r="B375" s="6" t="s">
+        <v>998</v>
+      </c>
+      <c r="C375" s="6" t="s">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="376" customFormat="false" ht="54.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A376" s="6" t="s">
+        <v>1000</v>
+      </c>
+      <c r="B376" s="6" t="s">
+        <v>1001</v>
+      </c>
+      <c r="C376" s="6" t="s">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="377" customFormat="false" ht="89.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A377" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="B377" s="6" t="s">
+        <v>1004</v>
+      </c>
+      <c r="C377" s="6" t="s">
+        <v>1005</v>
+      </c>
     </row>
     <row r="378" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A378" s="6"/>
+      <c r="A378" s="6" t="s">
+        <v>1006</v>
+      </c>
       <c r="B378" s="6"/>
-      <c r="C378" s="6"/>
+      <c r="C378" s="6" t="s">
+        <v>1007</v>
+      </c>
     </row>
     <row r="379" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A379" s="6"/>
@@ -9021,7 +9176,7 @@
   <sheetData>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="8" t="s">
-        <v>983</v>
+        <v>1008</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>2</v>
@@ -9033,10 +9188,10 @@
         <v>400</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>984</v>
+        <v>1009</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>985</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9044,10 +9199,10 @@
         <v>404</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>986</v>
+        <v>1011</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>987</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
feat: adding openApi problem representation model.
</commit_message>
<xml_diff>
--- a/src/main/resources/docs/especialista-spring-rest.xlsx
+++ b/src/main/resources/docs/especialista-spring-rest.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1087" uniqueCount="1013">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1091" uniqueCount="1017">
   <si>
     <t xml:space="preserve">Especialista Spring Rest</t>
   </si>
@@ -4660,7 +4660,33 @@
 De Acordo com Método HTTP</t>
   </si>
   <si>
+    <t xml:space="preserve">Podemos customizar as respostas de acordo com os metodos, 
+Com isso utilizamos o mesmo openApiCustomizer mas iteramos sobre os paths e filtramos pelos metodos:
+switch (httpMethod) {
+case GET:
+	responses.addApiResponse("404", new ApiResponse().description("Recurso não encontrado"));
+	break;
+case POST:
+responses.addApiResponse("400", new ApiResponse().description("Requisição inválida"));
+…</t>
+  </si>
+  <si>
     <t xml:space="preserve">26.13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Descrevendo Modelo do Problema</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Basta seguir o mesmo exemplo dos modelos e configurar no openApi Docs:
+@Schema(name = "Problema")
+public class Problem {…}
+Com isso teremos que registrar os schemas em openApi e depois referenciar em operations
+openApi...components(new Components().schemas(
+gerarSchemas()));
+@Operation(...@Content(schema = @Schema(ref = "Problema")))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26.14</t>
   </si>
   <si>
     <t xml:space="preserve">ERRO</t>
@@ -4795,7 +4821,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -4826,6 +4852,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -5023,7 +5053,7 @@
   <dimension ref="A1:F1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A376" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C379" activeCellId="0" sqref="C379"/>
+      <selection pane="topLeft" activeCell="B378" activeCellId="0" sqref="B378"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9078,19 +9108,27 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="378" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="378" customFormat="false" ht="119.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A378" s="6" t="s">
         <v>1006</v>
       </c>
-      <c r="B378" s="6"/>
+      <c r="B378" s="8" t="s">
+        <v>1007</v>
+      </c>
       <c r="C378" s="6" t="s">
-        <v>1007</v>
-      </c>
-    </row>
-    <row r="379" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A379" s="6"/>
-      <c r="B379" s="6"/>
-      <c r="C379" s="6"/>
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="379" customFormat="false" ht="109.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A379" s="6" t="s">
+        <v>1009</v>
+      </c>
+      <c r="B379" s="6" t="s">
+        <v>1010</v>
+      </c>
+      <c r="C379" s="6" t="s">
+        <v>1011</v>
+      </c>
     </row>
     <row r="380" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A380" s="6"/>
@@ -9175,225 +9213,225 @@
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="8" t="s">
-        <v>1008</v>
-      </c>
-      <c r="B2" s="8" t="s">
+      <c r="A2" s="9" t="s">
+        <v>1012</v>
+      </c>
+      <c r="B2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="9"/>
+      <c r="C2" s="10"/>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="9" t="n">
+      <c r="A3" s="10" t="n">
         <v>400</v>
       </c>
-      <c r="B3" s="9" t="s">
-        <v>1009</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>1010</v>
+      <c r="B3" s="10" t="s">
+        <v>1013</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>1014</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="9" t="n">
+      <c r="A4" s="10" t="n">
         <v>404</v>
       </c>
-      <c r="B4" s="9" t="s">
-        <v>1011</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>1012</v>
+      <c r="B4" s="10" t="s">
+        <v>1015</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>1016</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="9"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
+      <c r="A5" s="10"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="9"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
+      <c r="A6" s="10"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="9"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
+      <c r="A7" s="10"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="9"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
+      <c r="A8" s="10"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="9"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
+      <c r="A9" s="10"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="9"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
+      <c r="A10" s="10"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="9"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
+      <c r="A11" s="10"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="9"/>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
+      <c r="A12" s="10"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="9"/>
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
+      <c r="A13" s="10"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="9"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
+      <c r="A14" s="10"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="9"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
+      <c r="A15" s="10"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="9"/>
-      <c r="B16" s="9"/>
-      <c r="C16" s="9"/>
+      <c r="A16" s="10"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="9"/>
-      <c r="B17" s="9"/>
-      <c r="C17" s="9"/>
+      <c r="A17" s="10"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="9"/>
-      <c r="B18" s="9"/>
-      <c r="C18" s="9"/>
+      <c r="A18" s="10"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="9"/>
-      <c r="B19" s="9"/>
-      <c r="C19" s="9"/>
+      <c r="A19" s="10"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="9"/>
-      <c r="B20" s="9"/>
-      <c r="C20" s="9"/>
+      <c r="A20" s="10"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="10"/>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="9"/>
-      <c r="B21" s="9"/>
-      <c r="C21" s="9"/>
+      <c r="A21" s="10"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="9"/>
-      <c r="B22" s="9"/>
-      <c r="C22" s="9"/>
+      <c r="A22" s="10"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="9"/>
-      <c r="B23" s="9"/>
-      <c r="C23" s="9"/>
+      <c r="A23" s="10"/>
+      <c r="B23" s="10"/>
+      <c r="C23" s="10"/>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="9"/>
-      <c r="B24" s="9"/>
-      <c r="C24" s="9"/>
+      <c r="A24" s="10"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="10"/>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="9"/>
-      <c r="B25" s="9"/>
-      <c r="C25" s="9"/>
+      <c r="A25" s="10"/>
+      <c r="B25" s="10"/>
+      <c r="C25" s="10"/>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="9"/>
-      <c r="B26" s="9"/>
-      <c r="C26" s="9"/>
+      <c r="A26" s="10"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="10"/>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="9"/>
-      <c r="B27" s="9"/>
-      <c r="C27" s="9"/>
+      <c r="A27" s="10"/>
+      <c r="B27" s="10"/>
+      <c r="C27" s="10"/>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="9"/>
-      <c r="B28" s="9"/>
-      <c r="C28" s="9"/>
+      <c r="A28" s="10"/>
+      <c r="B28" s="10"/>
+      <c r="C28" s="10"/>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="9"/>
-      <c r="B29" s="9"/>
-      <c r="C29" s="9"/>
+      <c r="A29" s="10"/>
+      <c r="B29" s="10"/>
+      <c r="C29" s="10"/>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="9"/>
-      <c r="B30" s="9"/>
-      <c r="C30" s="9"/>
+      <c r="A30" s="10"/>
+      <c r="B30" s="10"/>
+      <c r="C30" s="10"/>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="9"/>
-      <c r="B31" s="9"/>
-      <c r="C31" s="9"/>
+      <c r="A31" s="10"/>
+      <c r="B31" s="10"/>
+      <c r="C31" s="10"/>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="9"/>
-      <c r="B32" s="9"/>
-      <c r="C32" s="9"/>
+      <c r="A32" s="10"/>
+      <c r="B32" s="10"/>
+      <c r="C32" s="10"/>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="9"/>
-      <c r="B33" s="9"/>
-      <c r="C33" s="9"/>
+      <c r="A33" s="10"/>
+      <c r="B33" s="10"/>
+      <c r="C33" s="10"/>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="9"/>
-      <c r="B34" s="9"/>
-      <c r="C34" s="9"/>
+      <c r="A34" s="10"/>
+      <c r="B34" s="10"/>
+      <c r="C34" s="10"/>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="9"/>
-      <c r="B35" s="9"/>
-      <c r="C35" s="9"/>
+      <c r="A35" s="10"/>
+      <c r="B35" s="10"/>
+      <c r="C35" s="10"/>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="9"/>
-      <c r="B36" s="9"/>
-      <c r="C36" s="9"/>
+      <c r="A36" s="10"/>
+      <c r="B36" s="10"/>
+      <c r="C36" s="10"/>
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="9"/>
-      <c r="B37" s="9"/>
-      <c r="C37" s="9"/>
+      <c r="A37" s="10"/>
+      <c r="B37" s="10"/>
+      <c r="C37" s="10"/>
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="9"/>
-      <c r="B38" s="9"/>
-      <c r="C38" s="9"/>
+      <c r="A38" s="10"/>
+      <c r="B38" s="10"/>
+      <c r="C38" s="10"/>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="9"/>
-      <c r="B39" s="9"/>
-      <c r="C39" s="9"/>
+      <c r="A39" s="10"/>
+      <c r="B39" s="10"/>
+      <c r="C39" s="10"/>
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="9"/>
-      <c r="B40" s="9"/>
-      <c r="C40" s="9"/>
+      <c r="A40" s="10"/>
+      <c r="B40" s="10"/>
+      <c r="C40" s="10"/>
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="9"/>
-      <c r="B41" s="9"/>
-      <c r="C41" s="9"/>
+      <c r="A41" s="10"/>
+      <c r="B41" s="10"/>
+      <c r="C41" s="10"/>
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="9"/>
-      <c r="B42" s="9"/>
-      <c r="C42" s="9"/>
+      <c r="A42" s="10"/>
+      <c r="B42" s="10"/>
+      <c r="C42" s="10"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
feat: adding openApi custom global responses.
</commit_message>
<xml_diff>
--- a/src/main/resources/docs/especialista-spring-rest.xlsx
+++ b/src/main/resources/docs/especialista-spring-rest.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1091" uniqueCount="1017">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1094" uniqueCount="1020">
   <si>
     <t xml:space="preserve">Especialista Spring Rest</t>
   </si>
@@ -4672,6 +4672,21 @@
   </si>
   <si>
     <t xml:space="preserve">26.13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Referenciando uma Respose</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Também podemos cira um mapa e fazer uma referência a ele:
+        apiResponseMap.put(internalServerErrorResponse, new ApiResponse()
+.description("Erro interno no servidor").content(content));
+…
+case DELETE:
+responses.addApiResponse("500", new ApiResponse().$ref(internalServerErrorResponse));
+ break;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26.15</t>
   </si>
   <si>
     <t xml:space="preserve">Descrevendo Modelo do Problema</t>
@@ -5052,8 +5067,8 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A376" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B378" activeCellId="0" sqref="B378"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A377" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B380" activeCellId="0" sqref="B380"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9119,21 +9134,27 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="379" customFormat="false" ht="109.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="379" customFormat="false" ht="89.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A379" s="6" t="s">
         <v>1009</v>
       </c>
-      <c r="B379" s="6" t="s">
+      <c r="B379" s="8" t="s">
         <v>1010</v>
       </c>
       <c r="C379" s="6" t="s">
         <v>1011</v>
       </c>
     </row>
-    <row r="380" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A380" s="6"/>
-      <c r="B380" s="6"/>
-      <c r="C380" s="6"/>
+    <row r="380" customFormat="false" ht="109.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A380" s="6" t="s">
+        <v>1012</v>
+      </c>
+      <c r="B380" s="6" t="s">
+        <v>1013</v>
+      </c>
+      <c r="C380" s="6" t="s">
+        <v>1014</v>
+      </c>
     </row>
     <row r="381" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A381" s="6"/>
@@ -9175,7 +9196,11 @@
       <c r="B388" s="6"/>
       <c r="C388" s="6"/>
     </row>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="389" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A389" s="6"/>
+      <c r="B389" s="6"/>
+      <c r="C389" s="6"/>
+    </row>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
@@ -9214,7 +9239,7 @@
   <sheetData>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>1012</v>
+        <v>1015</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>2</v>
@@ -9226,10 +9251,10 @@
         <v>400</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>1013</v>
+        <v>1016</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>1014</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9237,10 +9262,10 @@
         <v>404</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>1015</v>
+        <v>1018</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>1016</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
feat: adjuste representation models, inputs and pageable in openapi docs.
</commit_message>
<xml_diff>
--- a/src/main/resources/docs/especialista-spring-rest.xlsx
+++ b/src/main/resources/docs/especialista-spring-rest.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1094" uniqueCount="1020">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1097" uniqueCount="1023">
   <si>
     <t xml:space="preserve">Especialista Spring Rest</t>
   </si>
@@ -4686,7 +4686,7 @@
  break;</t>
   </si>
   <si>
-    <t xml:space="preserve">26.15</t>
+    <t xml:space="preserve">26.16</t>
   </si>
   <si>
     <t xml:space="preserve">Descrevendo Modelo do Problema</t>
@@ -4702,6 +4702,25 @@
   </si>
   <si>
     <t xml:space="preserve">26.14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Corrigindo Documentação com
+PageableParameter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Para representar parâmetros do tipo Pageable é necessário declarar vários parâmetros (page, size, sort)
+- Para melhorarmos a visibilidade e organização do código vamos criar uma anotação personalizada chamada PageableParameter
+- PageableParameter conterá todas as especificações e exemplos centralizados em uma única aotação:
+@Parameter(
+in = ParameterIn.QUERY,
+name = "sort",
+description = "Critério de ordenação: propriedade(asc|desc).",
+examples = { @ExampleObject("nome,desc") ...}
+)
+public @interface PageableParameter {...}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26.17</t>
   </si>
   <si>
     <t xml:space="preserve">ERRO</t>
@@ -5067,8 +5086,8 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A377" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B380" activeCellId="0" sqref="B380"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A367" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B385" activeCellId="0" sqref="B385"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9156,10 +9175,16 @@
         <v>1014</v>
       </c>
     </row>
-    <row r="381" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A381" s="6"/>
-      <c r="B381" s="6"/>
-      <c r="C381" s="6"/>
+    <row r="381" customFormat="false" ht="128.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A381" s="6" t="s">
+        <v>1015</v>
+      </c>
+      <c r="B381" s="6" t="s">
+        <v>1016</v>
+      </c>
+      <c r="C381" s="6" t="s">
+        <v>1017</v>
+      </c>
     </row>
     <row r="382" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A382" s="6"/>
@@ -9239,7 +9264,7 @@
   <sheetData>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>1015</v>
+        <v>1018</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>2</v>
@@ -9251,10 +9276,10 @@
         <v>400</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>1016</v>
+        <v>1019</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>1017</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9262,10 +9287,10 @@
         <v>404</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>1018</v>
+        <v>1021</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>1019</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
fix: removing old dependencies
</commit_message>
<xml_diff>
--- a/src/main/resources/docs/especialista-spring-rest.xlsx
+++ b/src/main/resources/docs/especialista-spring-rest.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1037" uniqueCount="968">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1194" uniqueCount="1101">
   <si>
     <t xml:space="preserve">Especialista Spring Rest</t>
   </si>
@@ -1276,6 +1276,9 @@
     <t xml:space="preserve">ResourceUtils.getContentFromResource("/json/correto/cozinha-chinesa.json")</t>
   </si>
   <si>
+    <t xml:space="preserve">10.8</t>
+  </si>
+  <si>
     <t xml:space="preserve">RestAssured</t>
   </si>
   <si>
@@ -1286,9 +1289,6 @@
     	&lt;artifactId&gt;rest-assured&lt;/artifactId&gt;
     	&lt;scope&gt;test&lt;/scope&gt;
     &lt;/dependency&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10.8</t>
   </si>
   <si>
     <t xml:space="preserve">Utilizando RestAssured</t>
@@ -3312,11 +3312,17 @@
 Authorization: Basic am9hbxzoxMjM=</t>
   </si>
   <si>
+    <t xml:space="preserve">22.1</t>
+  </si>
+  <si>
     <t xml:space="preserve">Spring Security</t>
   </si>
   <si>
     <t xml:space="preserve">- Apenas adicionando o Starter do Spring na nossa palicação já temos um formulário de login e senha
 - As próximas requisições serão autenticadas e precisarão do cabeçalho Authorization</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22.2</t>
   </si>
   <si>
     <t xml:space="preserve">Usuário e Senha Básicos</t>
@@ -3339,13 +3345,18 @@
     <t xml:space="preserve">WebSecurityConfig</t>
   </si>
   <si>
-    <t xml:space="preserve">- Classe de configuração WebSecurityque pode customizar as configurações de segurança
+    <t xml:space="preserve">- Classe de configuração WebSecurity que pode customizar as configurações de segurança
 - Pode definir quais endpoints serão autenticados ou não
 - Podemos definir estado da API como STATELESS para não guardarmos Cookies
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cross-Site Request Forgery</t>
+@EnableWebSecurity
+public class WebSecurityConfig extends WebSecurityConfigurerAdapter {…}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cross-Site Request Forgery
+CSRF</t>
   </si>
   <si>
     <t xml:space="preserve">- Conhecido como CSRF
@@ -3365,10 +3376,14 @@
 - Toda senha precisa ser criptografada por isso criaremos o methodo de encriptação passwordEncoder()</t>
   </si>
   <si>
+    <t xml:space="preserve">22.4</t>
+  </si>
+  <si>
     <t xml:space="preserve">OAuth2</t>
   </si>
   <si>
-    <t xml:space="preserve">- É um protocolo, é uma especificação
+    <t xml:space="preserve">'- Framework(Conjunto de regras) de segurança que utiliza http
+- É um protocolo, uma especificação
 - Mais usada para proteger APIs
 - Não trafega usuário e senha e sim Token de autorização
 - Servidor de Acesso retorna token em string e um cabeçalho precisa ser passado na requisição da API
@@ -3378,6 +3393,9 @@
 - Permite que APIs terceiras recebam acesso limitados a nossa aplicação usando protocolo HTTP</t>
   </si>
   <si>
+    <t xml:space="preserve">22.5</t>
+  </si>
+  <si>
     <t xml:space="preserve">Roles OAuth2</t>
   </si>
   <si>
@@ -3390,21 +3408,31 @@
     <t xml:space="preserve">Fluxo de Acesso</t>
   </si>
   <si>
-    <t xml:space="preserve">Resource Owner através do Client aciona o Authorization Server para garantir acesso ao Resource Server</t>
+    <t xml:space="preserve">- Resource Owner: Dono do Produto
+- Authorization Server: Porteiro, controlador do Acesso
+- Client: Aplicação que deseja acessar o Recurso ou seja acessar a API
+- Resource Server: API que contém os recursos
+Resource Owner através do Client aciona o Authorization Server para garantir acesso ao Resource Server
+O Cliente quer acessar o Resource Server em nome do Resource Owner e o Authorization Server que permite essa concessão
+O Client não quer o usuário e senha do Resource Owner, ele só solicita o acesso</t>
   </si>
   <si>
     <t xml:space="preserve">Resource Server</t>
   </si>
   <si>
     <t xml:space="preserve">- Podemos usar Spring Secuirity ou OAuth Server
-- OAuth Server está sendo depreciado e será migrado para Spring Security
+-  Spring Security OAuth  foi DEPRECIADO use apenas o  Spring Secuirity
 - Para que nossa aplicação passe a funcionar como um Resource Server é necessário uma dependência no pom.xml
 spring-boot-starter-oauth2-resource-server
 - Necessário customizar as configurações em ResourceServerConfig e especificar URI de checagem de token em application.properties
 - Após essa configuração é necessário passar no cabeçalho Authorization: Bearer + token (Bearer significa Titular)</t>
   </si>
   <si>
-    <t xml:space="preserve">Fluxo: Password Credentials Grant</t>
+    <t xml:space="preserve">22.6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fluxo: Resource Owner
+Password Credentials Grant</t>
   </si>
   <si>
     <t xml:space="preserve">- Garante um token a partir de um usuário e senha, também conhecido como Password Credentials
@@ -3414,6 +3442,9 @@
 OBS: Fluxo não aconselhado para ser usado, a não ser que não tenha outra solução</t>
   </si>
   <si>
+    <t xml:space="preserve">22.7</t>
+  </si>
+  <si>
     <t xml:space="preserve">Authorization Server Configurer Adapter</t>
   </si>
   <si>
@@ -3423,21 +3454,159 @@
 - Authorization Server produz o token para o Client e também valida o token quando o Resource Server o recebe.</t>
   </si>
   <si>
+    <t xml:space="preserve">22.8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Authorization Server Externo</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">AuthorizationServerConfig</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">: Extende AuthorizationServerConfigurerAdapter possui as definições necessária para a configuração do Servidor,
+Carrega a anotação @EnableAuthorizationServer e o método configure com os detalhes dos clients (memória ou banco de dados), 
+Podemos definir o fluxo (password, credentials, token) e scopes (read, write)
+Autenticacao para comunicacao com o server (no caso de querer consultar token security.checkTokenAccess("isAuthenticated()"))
+Podemos deixar como security.checkTokenAccess("permitAll()").tokenKeyAccess("permitAll()").allowFormAuthenticationForClients() pois é sóconsulta de token
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">WebSecurityConfig</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">: extende WebSecurityConfigurerAdapter e carrega a anotation @EnableWebSecurity possui PasswordEncode para criptografar as senhas e AuthenticationManager para gerenciar os usuários(Usado apenas no fluxo de “Password”)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">CorsConfig</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">: habilita o cors para que seja possível o fazer e receber requisições no authorization Server
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">PkceAuthorizationCodeTokenGranter</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">: Somente para caso for utilizar o fluxo PKCE
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">JwtCustomClaimsTokenEnhancer: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Para adicionar campos customizados no token JWT</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">22.9</t>
+  </si>
+  <si>
     <t xml:space="preserve">Requisição de Token</t>
   </si>
   <si>
     <t xml:space="preserve">- Requisição para /oauth/token
 - Authentication: Basic Client Credentials
-- Body: x-www-form com username, password e grant_type
+- Body: x-www-form com username, password e grant_type (username: jose, password: 123, grant_type: password)
 - Recebemos um token opaco: que é um token onde não sabemos as informações dele</t>
   </si>
   <si>
+    <t xml:space="preserve">Opaque Token</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Um token opaco é quando temos acesso ao token porém não conseguimos visualizar seu conteúdo
+Geralmente são representados em um formato UUID</t>
+  </si>
+  <si>
     <t xml:space="preserve">OAuth2 Introspection</t>
   </si>
   <si>
     <t xml:space="preserve">- Define o que deve ser passado na consulta e recebimento do Token do Authorization Server
-- A checkagem de token acontece na rota /oauth/check_token
+- A checkagem de token acontece na rota /oauth/check_token e indica se o token está ativo ou foi revogado
 - Configuração é definida por AuthorizationServerSecurityConfigurer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22.10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Authorization Server Interno</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Faz a checagem do token oauth2 no Resource Server
+Para isso definimos uma classe ResourceServerConfig extendendo WebSecurityAdapter
+@EnableWebSecurity
+public class ResourceServerConfig extends WebSecurityConfigurerAdapter {…}
+Com a configuração de instronspection-uri, client id e secret em application properties:
+spring.security.oauth2.resourceserver.opaquetoken.introspection-uri</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22.11</t>
   </si>
   <si>
     <t xml:space="preserve">Refresh Token</t>
@@ -3452,14 +3621,21 @@
 - Podemos invalidar um refresh token assim que usarmos uma vez com  .reuseRefreshTokens(false);</t>
   </si>
   <si>
+    <t xml:space="preserve">22.12</t>
+  </si>
+  <si>
     <t xml:space="preserve">Fluxo: Client Credentials Grant</t>
   </si>
   <si>
-    <t xml:space="preserve">- Quando uma aplicação gera token em nome dele própria e não em nome de algum usuário
+    <t xml:space="preserve">- Quando uma aplicação gera token em nome dela própria e não em nome de algum usuário
+- Normalmente uma aplicação backend acessando outra aplicação
 - Permite gerar um access token apenas com as credenciais do client
 - Usa no gant type: client_credentials
 - Não permite usar refresh_token
 - Para configura-lo basta criar um novo client em AuthorizationServerConfig</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22.15</t>
   </si>
   <si>
     <t xml:space="preserve">Fluxo: Authorization Code Grant</t>
@@ -3474,38 +3650,54 @@
 - Para chamar a API é necessário informar no cabeçalho o code recebido, o grant_type como authorization_code e redirect_uri sendo a url definida http://aplicacao-cliente</t>
   </si>
   <si>
+    <t xml:space="preserve">22.18</t>
+  </si>
+  <si>
     <t xml:space="preserve">Fluxo: Implicit Grant</t>
   </si>
   <si>
-    <t xml:space="preserve">- Semelhante ao Authorization Code porém simplificado (LEGADO: Esse fluxo não deve ser usado)
-- Ao invés de retornar um código já retorna o token na URL
+    <t xml:space="preserve">- Semelhante ao Authorization Code porém simplificado (LEGADO: Esse fluxo não deve ser usado, segurança fraca)
+- Ao invés de retornar um código já retorna o token na URL (Não emite refresh token)
+Utiliza authorizedGrantTypes(“implicit”)
 http://auth.algafood.local:8081/oauth/authorize?response_type=token&amp;client_id=webadmin&amp;state=abc&amp;redirect_uri=http://aplicacao-cliente
 - Implicit não emite refresh token</t>
   </si>
   <si>
+    <t xml:space="preserve">22.20</t>
+  </si>
+  <si>
     <t xml:space="preserve">Authorization Code + PKCE</t>
   </si>
   <si>
     <t xml:space="preserve">- Proof Key for Code Exchange (Chave de Prova para Troca de Código)
+- É uma extensão do OAuth2
 - Resolve fluxo de clientes públicos, onde não é possível manter a confidencialidade das credenciais (client_id e client_secret de fácil acesso)
+IMPORTANTE: não necessita que client_id e secret sejam expostos no código, pois utiliza um certificado
 - Token só será fornecido após validação do Code Challenge em SHA-256 e Bae64 Url
-1° - Client gera Verifier e Code Challange, então Autorization Server mantém o código para validação futura
-2° - Solicita a aprovação passando o code_challange e vefifier
-- No momento de solicitar o acesso token é passado o code, grant_type e redirect_uri passando o verifyer para validação do code_challenge
+1° - Client gera Verifier e Code Challange(SHA-256), então Autorization Server mantém o código para validação futura
+2° - Solicita a aprovação passando o code_challange e verifier
+- No momento de solicitar o acesso token é passado o code, grant_type e redirect_uri passando o verifier para validação do code_challenge
+(Code chalenge só será utilizado nesse passo para autenticar com o Authorization Server)
 Para implementá-lo usamos o método tokenGranter
 - O tokenGranter instancia o Authorization Code com PKCE
 Exemplo de Url de Authenticação:
 http://auth.algafood.local:8081/oauth/authorize?response_type=code&amp;client_id=foodanalytics&amp;state=abc&amp;redirect_uri=http://aplicacao-cliente&amp;code_challenge=teste123&amp;code_challenge_method=plain
 3° - Depois de Autenticado e aprovado, faremos uma nova requisição porém agora passando o code_challenge no cabeçalho do code_verifier e então recebemos um token
 4º – Seguimos com a chamada à aplicação
-Evita ataques de força bruta pois tem somente uma chance para acertar o code_challenge, caso errar o code_cerifier será invalidado.</t>
+OBS.: Evita ataques de força bruta pois tem somente UMA chance para acertar o code_challenge, caso errar o code_cerifier será invalidado.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22.22</t>
   </si>
   <si>
     <t xml:space="preserve">Clientes Público x Confidencial</t>
   </si>
   <si>
-    <t xml:space="preserve">- Público é aquele que tem o client_id exposto, mesmo que compilado como no caso dos mobile, é possível fazer uma engenharia reversa e resgatar esse código
+    <t xml:space="preserve">- Público é aquele que tem o client_id exposto, mesmo que compilado como no caso dos mobile ou web(SPA), é possível fazer uma engenharia reversa e resgatar esse código
 - Confidencial: Comunicação com o Authorization é feita no Servidor e não no Browser como usuário final</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22.27</t>
   </si>
   <si>
     <t xml:space="preserve">Clientes Confiáveis x Não Confiáveis</t>
@@ -3533,6 +3725,24 @@
 - Configurado a partir do AuthorizationServerEndpointsConfigure</t>
   </si>
   <si>
+    <t xml:space="preserve">23.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RedisToken Store</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'- Armazenamento de token no store do Redis
+- Adicionar no Authorization Server a dependência starter no spring: spring-boot-starter-data-redis
+- Configurar properties com host, port e password
+- Configurar endpoint server para armazenamento no redis na classe AuthorizationServerConfig:
+@Override public void configure(AuthorizationServerEndpointsConfigurer endpoints) throws Exception {…}
+endpoints...tokenStore(new RedisTokenStore(redisConnectionFactory))
+	.tokenGranter(tokenGranter(endpoints));</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23.2</t>
+  </si>
+  <si>
     <t xml:space="preserve">Statefull vs Stateless</t>
   </si>
   <si>
@@ -3542,12 +3752,15 @@
  e não precisar armazenar informações no servidor. (Referindo-se ao estado da Aplicação e não dos Recursos)</t>
   </si>
   <si>
+    <t xml:space="preserve">23.3</t>
+  </si>
+  <si>
     <t xml:space="preserve">Application State vs Resource State</t>
   </si>
   <si>
     <t xml:space="preserve">- Estado da Aplicação e Estado dos Recursos
 - Estado dos Recursos são relacionados aos domínios do negócio (Cozinhas, Restaurantes e Etc)
-- Estado da aplicação é o mesmo que o estado da Sessão do Usuário, (Cliente é força a fazer várias requisições)</t>
+- Estado da aplicação é o mesmo que o estado da Sessão do Usuário (Cliente é força a fazer várias requisições)</t>
   </si>
   <si>
     <t xml:space="preserve">Statefull Authentication vs Stateless Authentication</t>
@@ -3560,40 +3773,70 @@
 * Ultiliza Transparent Token, tem informações do usuário contidas no token
 * Resolve as desvantagens do Statefull
 * Sessão do Usuário armazenada no lado do cliente
-* Servidor não sabe qauis tokens emitiu, apenas consegue validá-los
+* Servidor não sabe quais tokens emitiu, apenas consegue validá-los
 * Token só revoga após a expiração do tempo definido </t>
   </si>
   <si>
     <t xml:space="preserve">Trasparent Token</t>
   </si>
   <si>
-    <t xml:space="preserve">- É um token composto por Header, payload e assinatura
-- Possui o formato de uma string Encodada em base 64
+    <t xml:space="preserve">- Um transparente token refere-se a um token de autenticação que é gerado, validado e transmitido sem necessidade de intervenção do usuário, permitindo acesso contínuo e seguro a recursos protegidos.
+- NÃO PRECISA ARMAZENAR AS INFORMAÇÕES EM SERVIDOR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Json Web Token
+JWT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- JWT é um tipo de token transparente com formato json padrão
+- Transporta dados de uma forma compacta e segura
+- Possui uma string criptografada em Base64 e assinado com um HASH criptografico
+- Possui 3 partes: Header, Payload, e Assinatura
 - Para decodificar o token podemos usar o site:
 http://jwt.io
 - O Header é um objeto json que possui informações como tipo do token e tipos de criptografia usada
 - O Payload possui informações (CLAIM) de autorização e autenticação com o Servidor
 - Assinatura: informações de criptografia
 - O tamanho da senha precisa ser 32 bit.
+- IMPORTANTE: Só quem possui a chave consegue criptografar e descriptografar o token, essa chave não é fornecida na requisição mas ambos os lados conhecem
+- Dependência: spring-security-jwt
 - Para visualizar problemas com Token habilite o log level DEBUG:
-logging.level.org.springframework=DEBUG
-- NÃO PRECISA ARMAZENAR AS INFORMAÇÕES EM SERVIDOR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Criptografia Simétrica</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- Usa uma chave compartilhada por que emite e receber uma mensagem (SHMA).
-- Authorization Server compartilha cave com Resource Server.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Criptografia Assimétrica</t>
+logging.level.org.springframework=DEBUG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Criptografia Simétrica
+SHA256</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Usa uma chave compartilhada por quem emite e receber uma mensagem (SHMA).
+- Ou Seja, ambos os lados possuem a chave e ela não é trafegada na requisição
+- Authorization Server compartilha cave com Resource Server.
+- NÃO É NECESSÁRIO ARMAZENAR NENHUM TOKEN
+@Bean
+public JwtAccessTokenConverter jwtAccessTokenConverter() {
+	var jwtAccessTokenConverter = new JwtAccessTokenConverter();
+	jwtAccessTokenConverter.setKeyPair("CHAVE_SIMETRICA");
+	return jwtAccessTokenConverter;
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Criptografia Assimétrica
+RS256</t>
   </si>
   <si>
     <t xml:space="preserve">- Utiliza um par de chaves, sendo uma privada e a outra pública (RS256)
-- Emissor possui a chave privada, Autorization deve possui uma chave e não compartilhá-la com ninguém
+- Emissor possui a chave privada, Autorization deve possuir uma chave e não compartilhá-la com ninguém
 - Chave privada é que assina o JWT.
-- Receptor usa chave pública, Resource Server só valida a assinatura, é aberta, se interceptar não tem problema.</t>
+- Receptor usa chave pública, Resource Server SÓ valida a assinatura, é aberta, se interceptar não tem problema.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23.7</t>
   </si>
   <si>
     <t xml:space="preserve">KeyTool</t>
@@ -3603,12 +3846,58 @@
 - Já está contida no JDK
 - Cria e Gerencia arquivos JKS (Repositório para Armazenar um Conjunto de Chaves Criptograficas em Formato Binário)
 Criando Chaves:
-keytool -genkeypair -alias algafood -keyalg RSA -keypass 123456 -keystore algafood.jks -storepass 123456
+keytool -genkeypair -alias algafood -keyalg RSA -keypass CHAVE_PRIVADA -keystore algafood.jks -storepass SENHA_DO_ARQUIVO
 Keypass: senha do par de chaves
 Storepass: Senha do Arquivo JKS
 Keyalg: Algoritmo usado
 Listar Entradas:
 keytool -list -keystore algafood.jks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23.8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Configurar Auth Server
+ para assinar com JKS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- O ideal é ter um par de chaves JKS para cada ambiente DEV e PROD
+- JKS será usado para assinar o token
+- Dentro de um arquivoo JKS podem conter vários pares de chaves, que são definidos por um alias
+- Alteramos o JwtAccessTokenConverter para utilizar o arquivo JKS:
+...jwtAccessTokenConverter() {	
+	var jksResource = new ClassPathResource(jwtKeyStoreProperties.getPath());
+	var keyStorePass = jwtKeyStoreProperties.getPassword();
+	var keyPairAlias = jwtKeyStoreProperties.getKeypairAlias();
+	var keyStoreKeyFactory = new KeyStoreKeyFactory(jksResource, keyStorePass.toCharArray());
+	var keyPair = keyStoreKeyFactory.getKeyPair(keyPairAlias);
+	jwtAccessTokenConverter.setKeyPair(keyPair);
+	return jwtAccessTokenConverter;
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23.9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Configurar Resource Server 
+Para validar token</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- A partir do JKS extraimos um certifica .PEM
+- Esse certificado contém a chave publica para validação da assinatura do JWT
+- Esse arquivo possui o formato texto criptografado
+Para validarmos no Resorce Server devemos configurar para que ao receber a requisição seja interceptado e extraída essas informações:
+- Configuramos nosso properties apontando o local da chave pública:
+#spring.security.oauth2.resourceserver.jwt.public-key-location=classpath:keys/algafood-pkey.pem
+- Na classe ResourceServerConfig vamos configurar o metodo configure:
+... configure(HttpSecurity http) throws Exception {
+http...oauth2ResourceServer().jwt()
+.jwtAuthenticationConverter(jwtAuthenticationConverter());
+}
+- A função jwtAuthenticationConverter devemos cria-la de forma que possamos descriptografar o token e extrair as permissões necessárias dele.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23.11</t>
   </si>
   <si>
     <t xml:space="preserve">Certificado .pem</t>
@@ -3646,23 +3935,104 @@
     <t xml:space="preserve">Aprovação Granular</t>
   </si>
   <si>
-    <t xml:space="preserve">- Com as alterações a aprovação de acesso no login da nossa aplicação passa a ser mais encapsulada e generalizada
-- Caso queira um aprovação Granular de certos recursos utilize um TokenApprovalStore no Authorization Server Config</t>
+    <t xml:space="preserve">- A aprovação granular permite que seja definidos escopoes no momento da aprovação, read ou write 
+- Com as alterações a aprovação de acesso no login da nossa aplicação passa a ser mais encapsulada e generalizada
+- Caso queira um aprovação Granular de certos recursos utilize um TokenApprovalStore no Authorization Server Config
+- A ordem como é cofigurada tem relevância ou seja gere o token primeiro e em seguida adicione um Approval Token:
+.tokenEnhancer(enhancerChain)
+	.approvalStore(approvalStore(endpoints.getTokenStore()))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23.12</t>
   </si>
   <si>
     <t xml:space="preserve">UserDetailsService</t>
   </si>
   <si>
-    <t xml:space="preserve">- Serviço para exposição de Usuários do Banco com o propósito de usá-los para autenticação do Resource</t>
+    <t xml:space="preserve">'- Serviço para exposição de Usuários do Banco com o propósito de usá-los para autenticação do Resource
+- Para configurar a utilização de usuários do banco de dados na autenticação necessitamos ajustar nosso Authorization Server:
+- Primeiro as dependências do JPA, MySQL e Lombook
+- Depois Repositórios, Entidades e JpaUserDetailsService
+- Em JpaUserDetailService é necessário implementar o método loadUserByUsername para buscar o usuário que vamos autenticar
+- Lembrando que a senha deve estar encriptografada para ser utilizada, podemos usar o Password Encoder
+- Definir as configurações do Server
+@Override
+...configure(AuthorizationServerEndpointsConfigurer endpoints) throws Exception {
+endpoints
+.authenticationManager(authenticationManager)
+.userDetailsService(userDetailsService)
+.authorizationCodeServices(new JdbcAuthorizationCodeServices(this.dataSource)…}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23.14</t>
   </si>
   <si>
     <t xml:space="preserve">Claim JWT</t>
   </si>
   <si>
-    <t xml:space="preserve">- Claim são os tributos do json JWT
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">- Claim são os tributos do json JWT
 - Podemos adicionar novos cliams no nosso token
-- Para isso criamos uma classe JwtCustomClaimsTokenEnhance
-- Podemos trafegar informações do Usuário, Nome Completo, e-mail, id</t>
+- Para isso criamos uma classe </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">JwtCustomClaimsTokenEnhancer
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">- Podemos trafegar informações do Usuário, Nome Completo, e-mail, id</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">23.16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">enhancerChain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Uma cadeia de claims que são oincrementadas ao token
+- Usamos o JwtCustomToken para adicionar as propriedades customizadas e o jwtAccessToken para adicionar informações do acesso
+var enhanceChain = new TokenEnhancerChain();
+enhanceChain.setTokenEnhancers(
+Arrays.asList(new JwtCustomClaimsTokenEnhancer(), jwtAccessTokenConverter()));
+- Depois ajustamos o token no configure
+endpoins....tokenEnhancer(enhancerChain)...</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Informações de Usuário Logado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Podemos obter as informações do usuário logado através do token que recebemos na requisição
+- Através do jwtCustomClaims definimos email, nome e id do usuário
+- Podemos então atribuir um pedido ao usuário logados, restringir seus acessos a determinados endpoint
+- Tudo isso através das informações obtidas pelo token
+Exemplo:
+novoPedido.getCliente().setId(algaSecurity.getUsuarioId());
+public Long getUsuarioId(){
+	Jwt jwt = (Jwt) getAuthentication().getPrincipal();
+Return jwt.getClaim("usuario_id");}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23.17</t>
   </si>
   <si>
     <t xml:space="preserve">Permissoes</t>
@@ -3671,7 +4041,26 @@
     <t xml:space="preserve">- Para acrescentar as permissões dos usuários usaremos a classe AuthUser com a seguinte definição:
 Collection&lt;? extends GrantedAuthority&gt; autorities
 - E em JpaUserDetailService usaremos SimpleGrantedAuthority para definir as permissões.
-- É necessário extrair as permissões do token JWT usando jwtAuthenticationConverter.</t>
+- É necessário extrair as permissões do token JWT usando jwtAuthenticationConverter.
+usuario.getGrupos().stream()
+.flatMap(grupo -&gt; grupo.getPermissoes().stream())
+			.map(permissao -&gt; new SimpleGrantedAuthority(permissao.getNome().toUpperCase()))
+.collect(Collectors.toSet());</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23.19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jwtAuthenticationConverter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Devemos converter cada String recebida com os nomes de permissões em um objeto de Permissões
+- Para isso usamos o jwtAuthenticationConverter() e setamos nas configurações do http:
+http....oauth2ResourceServer().jwt()
+				.jwtAuthenticationConverter(jwtAuthenticationConverter());</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23.20</t>
   </si>
   <si>
     <t xml:space="preserve">Method Security</t>
@@ -3686,6 +4075,33 @@
 @CheckSecurity.Cozinhas.PodeEditar</t>
   </si>
   <si>
+    <t xml:space="preserve">23.21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MetaAnotações</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Funcionam como expressões dentro de uma anotação
+- Uma Meta Anotação carrega propriedades de uma ou mais anotação que se resolvem através de um metodo
+Exemplo:
+@CheckSecurity.Cozinhas.PodeConsultar
+@GetMapping(value = "/{cozinhaId}")
+public CozinhaModel buscar(@PathVariable Long cozinhaId) {…}
+- Temos a meta anotação @CheckSecurity.Cozinhas.PodeConsultar que faz a verificação das permissões e defini se podemos ou não ulitizar aquele metodo do controlador
+public @interface CheckSecurity {…} com 
+@PreAuthorize("@algaSecurity.podeConsultarCozinhas()")
+        @Retention(RUNTIME)
+        @Target(METHOD)
+        public @interface PodeConsultar { }
+Aqui é chamado um metodo que retorna um valoo booleano dizendo se tem ou não aquela permissão:
+@algaSecurity.podeConsultarCozinhas()
+public boolean podeConsultarCozinhas() {
+	    return isAutenticado() &amp;&amp; temEscopoLeitura();}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23.23</t>
+  </si>
+  <si>
     <t xml:space="preserve">Scope Security</t>
   </si>
   <si>
@@ -3695,14 +4111,22 @@
 @PreAuthorize("hasAuthority('SCOPE_WRITE') and hasAuthority('EDITAR_COZINHAS')")</t>
   </si>
   <si>
+    <t xml:space="preserve">23.24</t>
+  </si>
+  <si>
     <t xml:space="preserve">@PostAuthorize</t>
   </si>
   <si>
     <t xml:space="preserve">- Realiza uma verificação após o método ser chamado
 - Deve ser usado para casos onde não gere efeitos colaterais
 - Podemos usar variaveis implicitas pois o método já foi executado e retornou alguma informação
+- IMPORTANTE: Como fazemos a consulta do pedido podemos checar se o retorno desse pedido pertence a ele, 
+é útil porque só realiza a query apenas uma vez e aproveita o retorno para fazer uma outra verificação
 - Um exemplo de variavel implicita é o returnObject que é o retorno do methodo
 @PostAuthorize("hasAuthority('CONSULTAR_PEDIDOS') or @algaSecurity.getUsuarioId() == returnObject.cliente.id")</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23.29</t>
   </si>
   <si>
     <t xml:space="preserve">Autenticação por Banco de Dados</t>
@@ -3711,9 +4135,15 @@
     <t xml:space="preserve">- Talvez seja necessário a criação de uma tablea para armazenar as aplicações que farão a solicitação de Token
 - Para isso setamos a configuração do Authorization Server para buscar os dados de acesso
 - Em ClientDetailsServiceConfigurer configuraremos os clients como jdbc
+@Override
+public void configure(ClientDetailsServiceConfigurer clients) throws Exception {
+clients.jdbc(dataSource);}
 - Para debugar possíveis erros utilizar:
 logging.level.org.springframework=DEBUG
 - Também é necessário a criação da tabela oauth_client_details</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23.36</t>
   </si>
   <si>
     <t xml:space="preserve">Tabela OAUTH_CLIENT_DETAILS</t>
@@ -3730,44 +4160,107 @@
 Authorities: define authorities padrão para o toke ‘EDITAR_COZINHAS,EDITAR_RESTAURANTES’ </t>
   </si>
   <si>
+    <t xml:space="preserve">23.37</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Juntando o Authorization Server 
+dentro do Resource Server</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Possui vantagens como economia de custos em instancias de aplcação em nuvem
+- Para escalabilidade de serviço
+- Adicione as dependências de segurança no projeto e traga as classes do Authorization Server para Resource Server
+- WebSecurity,AuthUser, CorsConfig, e as Classes do JWT
+- Arquivo jks e suas propriedades definidas em application.properties</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23.41</t>
+  </si>
+  <si>
     <t xml:space="preserve">SecurityScheme</t>
   </si>
   <si>
-    <t xml:space="preserve">- Para que seja opossível executar testes em nossa API através da documentação é necessário o securityScheme
+    <t xml:space="preserve">- Para que seja possível executar testes em nossa API através da documentação é necessário o securityScheme
 - Configurado no SpringFoxConfig ele tem como objetivo especificar o metodo de segurança usado na API
 - Ao configura-lo um botão de Authorize será exibido na documentação.</t>
   </si>
   <si>
+    <t xml:space="preserve">23.42</t>
+  </si>
+  <si>
     <t xml:space="preserve">Customização de Tela de Login</t>
   </si>
   <si>
-    <t xml:space="preserve">'- Podemos Customizar a tela de Login usada para autenticação da nossa API:
+    <t xml:space="preserve">'- ThymeLeaf é uma templete Engine do Java para criar páginas dinâmicas
+- Podemos Customizar a tela de Login usada para autenticação da nossa API:
 http://api.algafood.local:9000/login
 - Precisamos adicionar a dependecia do Thymeleaf
-_x0001_&lt;dependency&gt;
-&lt;groupId&gt;org.springframework.boot&lt;/groupId&gt;
-&lt;artifactId&gt;spring-boot-starter-thymeleaf&lt;/artifactId&gt;
-&lt;/dependency&gt;
-- ThymeLeaf é uma templete Engine do Java para criar páginas dinâmicas</t>
+spring-boot-starter-thymeleaf
+- Definimos o path do login em ResourceServerConfig
+...configure(HttpSecurity http) throws Exception {
+http.formLogin().loginPage("/login")... }
+- Criar um controlador para receber a requisição no path definido
+@Controller
+public class SecurityController {
+@GetMapping("/login")
+public String login() {return "pages/login";}}
+- Colocar os arquivos de paginas em resources/templates/pages/login.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23.43</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Customização de 
+Pagina de Aprovação OAuth2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Pagina que define escopo de aprovação sendo READ e/ou WRITE
+- Para customiza-la insira os arquivos na pasta resources/template/pages
+- Capture a requisição para redirecionar o acesso:
+	@GetMapping("/oauth/confirm_access")
+public String approval() {return "pages/approval";}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23.44</t>
   </si>
   <si>
     <t xml:space="preserve">Proteção de Arquivos de Keys</t>
   </si>
   <si>
-    <t xml:space="preserve">- Para Securança da nossa aplicação tempos chaves de Acesso JKS e o Certificado PEM
-- Caso queira subir para produção essa chaves não devem ser expostas por motivos de Segurança
+    <t xml:space="preserve">- Para Segurança da nossa aplicação temos chaves de Acesso JKS e o Certificado PEM
+- Caso queira subir para produção essa chaves NÃO devem ser expostas por motivos de Segurança
 - Para isso devemos substituir por JWKS (Json Web Key Set)</t>
   </si>
   <si>
+    <t xml:space="preserve">23.45</t>
+  </si>
+  <si>
     <t xml:space="preserve">Json Web Key Security</t>
   </si>
   <si>
     <t xml:space="preserve">- Conjunto de Chaves contendo as chaves públicas usadas para verificar os JWTs emitidos pelo Authorization Server e Assinados pelo SHA256
-- Criaremos um endpoint que irá gerar um conjunto de chaves para acesso públicas para usarmos
-- Para isso no AuthorizationServerConfig criaremos um método que para resgatar a chave pública JWKSet e expomos com @Bean
+- Criaremos um endpoint que irá gerar um conjunto de chaves para acesso públicas para usarmos e
+deletamos o arquivo PEM (chave publica) da nossa pasta
+- No AuthorizationServerConfig criaremos um método que para resgatar a chave pública JWKSet e expomos com @Bean
+@Bean public JWKSet jwkSet() {…}
+private KeyPair keyPair() {…}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Endpoint JKS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
 - O Endpoint precisará tem como URI o valor “.well-known/jwks.json”
 - Para expor o Endpoint criaremos um controlador JwKSetController expondo a URI citada e também acrescentar no application properties:
-spring.security.oauth2.resourceserver.jwt.jwk-set-uri=http://localhost:9000/.well-known/jwks.json</t>
+spring.security.oauth2.resourceserver.jwt.jwk-set-uri=http://localhost:9000/.well-known/jwks.json
+@RestController
+public class JwkSetController {
+@Autowired
+private JWKSet jwkSet;
+@GetMapping("/.well-known/jwks.json")
+public Map&lt;String, Object&gt; keys(){
+return this.jwkSet.toJSONObject();
+}}</t>
   </si>
   <si>
     <t xml:space="preserve">Externalizar o JKS</t>
@@ -3776,10 +4269,21 @@
     <t xml:space="preserve">- Implementar um Protocolo para carregar o Resource em Base 64 no application.properties
 - comando para retornar o jks em base64
 cat algafood.jks | base64 (No Linux) ou por algum site que converta em base64
-- Ao converter o arquivo para base¨4 e salvar no aplication.properties precisamos de uma classe que resolva essa codificação
+- Ao converter o arquivo para base64 e salvar no aplication.properties precisamos de uma classe que resolva essa codificação
+algafood.jwt.keystore.jks-location=base64:MIIKqAIBAzCCClIGCSqGSIb3DQEHA…
 - Criaremos a classe Base64ProtocolResolver para ler o arquivo.
+public class Base64ProtocolResolver implements ProtocolResolver,ApplicationListener&lt;ApplicationContextInitializedEvent&gt;{...}
+-Para fazer a leitura:
+var keyStoreKeyFactory = new KeyStoreKeyFactory(jwtKeyStoreProperties.getJksLocation(), keyStorePass.toCharArray());
 - Precisamos instanciar um listener para subir com o contexto do Spring implementando tambem ApplicationListener
-- E por fim adicionamos antes de iniciar a aplicação no ApplicationSpring.</t>
+Com isso o Spring saberá resolver o Base64 em properites
+- E por fim adicionamos antes de iniciar a aplicação no ApplicationSpring.
+var app = new SpringApplication(AlgafoodApiApplication.class);
+app.addListeners(new Base64ProtocolResolver());
+app.run(args);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23.46</t>
   </si>
   <si>
     <t xml:space="preserve">Docker</t>
@@ -4451,6 +4955,302 @@
   </si>
   <si>
     <t xml:space="preserve">26.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Removendo SpringFox</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O SpringDoc não funciona em conjunto com SpringFox
+Para remover as dependências do SpringFox devemos remover do pom.xml o spring-fox-bean-validator e springfox-swagger-ui</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adicionando SpringDoc no Projeto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adicione as seguintes dependências ao projeto:
+Springdoc-openapi-ui, springdoc-openapi-hateoas e springdoc-openapi-security
+Todos na versao 1.6.9 com Spring na versão 2.7.1 e java 17
+Com isso é possível acessar a documentacao em swagger-ui/index.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bean OpenApi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No Bean do OpenApi estão as configurações de inicialização do swagger
+Estão as configurações que podemos customizar:
+@Configuration
+public class SpringDocConfig {…}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Limitando presença de Controllers na Documentação</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Faz com que seja possível limitar quais os pacotes serão escaneados para apresentação da documentação
+Em application.properties insira a configuração:
+springdoc.packages-to-scan=com.algaworks.algafood.api
+Também podemos limitar a descoberta por paths:
+springdoc.path-to-match=/v1/**,/v2/**</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bean GroupedOpenApi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Utilizado para fazer separações na documentação entre versionamentos de controladores
+- Criamos um Bean para agrupar todos os controllers de uma versão:
+@Bean
+public GroupedOpenApi v1Api() {
+return GroupedOpenApi.builder()
+.group("v1")
+.pathsToMatch("/v1/**")
+.build();
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Segurança na Documentação
+Botão Authorize</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Para realizar autenticação na documentação para envio de requisições usamos a anotação @SecurityScheme
+@Configuration
+@SecurityScheme(name = "security_auth", type = SecuritySchemeType.OAUTH2)@Configuration
+@SecurityScheme(
+name = "security_auth",
+type = SecuritySchemeType.OAUTH2,
+flows =  @OAuthFlows(authorizationCode = @OAuthFlow(
+authorizationUrl = "${springdoc.oAuthFlow.authorizationUrl}",
+tokenUrl = "${springdoc.oAuthFlow.tokenUrl}",
+scopes = {
+@OAuthScope(name = "READ", description = "read scope"),
+@OAuthScope(name = "WRITE", description = "write scope"),
+}
+)))
+Public class SpringDocConfig {…}
+- Com isso um botão de Authorize aparecerá ao canto da tela para autenticar seu usuário para requisições
+- Crie as chaves no application.properties e configura a autenticação
+springdoc.oAuthFlow.authorizationUrl=http://localhost:9000/oauth/authorize
+springdoc.oAuthFlow.tokenUrl=http://localhost:9000/oauth/token</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Preparando Autorização</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Definir o client para preenchimento automático:
+springdoc.swagger-ui.oauth.client-id=algafood-web
+springdoc.swagger-ui.oauth.client-secret=web123
+E utilizaça o do PKCE:
+springdoc.swagger-ui.oauth.use-pkce-with-authorization-code-grant=true
+- Em oauth_client_details adicione o redirecionamento e permissões do usuário
+Na coluna ‘scope’ deve conter: 
+  'READ,WRITE', 'password,authorization_code', 'http://localhost:9000,http://localhost:9000/swagger-ui/oauth2-redirect.html', null,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adiciona no Controllers a Anotação de Segurança</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Para autorização do fluxo que implementamos é necessário adicionar uma anotação sobre os controladores com o nome da security que criamos
+@SecurityRequirement(name="security_auth")
+public interface CidadeControllerOpenApi {…}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Autorizando</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ao clicar no botão ao canto da tela em documentação é possível observar que tudo está preenchido e configurado
+Selecione todos os escopos e clique em autorizar
+Preencha com as credenciais de seu usuário joao.ger@algafood.com.br</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Criação de TAGs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Servem para agrupar alguns recursos semelhantes definindo nome e descrição
+@Tag(name = "Cidades", description = "Gerencia as Cidades")
+public interface CidadeControllerOpenApi {…}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26.6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Descrevendo Operações</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Descreve uma aoperação de um endpoint na documentação:
+	@Operation(summary = "Cadastra uma cidade", description = "Cadastro de uma cidade, necessita de um estado e um nome válido")
+	CidadeModel adicionar(CidadeInput cidadeInput);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26.7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Descrevendo Parâmetros</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Define os parâmetros nos recursos attravés da anotação @Parameter e também @Requestbody do swagger
+Também é possível definir um exemplo que autocompletará na documentação:
+CidadeModel buscar(@Parameter(description = "ID de uma cidade", example = "1", required = true) Long cidadeId);
+	CidadeModel adicionar(@RequestBody(description = "Representação de uma nova cidade", required = true) CidadeInput cidadeInput);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26.8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Descrevendo Modelos de Representação</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Podemos descrever os Modelos de Representação, seus campos e classes
+- Essa configuração é refletida tanto requisição quanto nos modelos representados abaixo na documentação
+@NotBlank
+@Schema(example = "Uberlândia")
+private String nome;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26.9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Descrevendo Validação de Modelo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Para definir as validações de modelo o springDocs consegue aproveitar as anotações já definidas como @NotBlank, @NotNull
+- Mas podemos definir na própria anotação caso necessário com required = true
+- Porém é preferível continuar utilizando as anotações do Javax
+@Schema(example = "Uberlândia", required = true)
+private String nome;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26.10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Definindo Códigos de Respostas 
+De Forma Global</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Necessário a criação de um Bean OpenAPICustomizer
+Essa customização faz um iteração sobre os paths da nossa aplicação e adiciona ApiResponse Globeis nele de acordo com seus status
+                        ApiResponse apiResponseNaoEncontrado = new ApiResponse().description("Recurso não encontrado");
+                        responses.addApiResponse("406", apiResponseNaoEncontrado);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26.11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Descrevendo StatusCode 
+Para Respostas Específicas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Na anotação de @Operation basta passar o código e descrição
+	@Operation(summary = "Busca uma cidade por Id", responses = {
+			@ApiResponse(responseCode = "200"),
+			@ApiResponse(responseCode = "400", description = "ID da cidade inválido",
+					content = @Content(schema = @Schema))})
+	CidadeModel buscar(@Parameter(description = "ID de uma cidade", example = "1", required = true) Long cidadeId);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26.12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Descrevendo StatusCode
+De Acordo com Método HTTP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Podemos customizar as respostas de acordo com os metodos, 
+Com isso utilizamos o mesmo openApiCustomizer mas iteramos sobre os paths e filtramos pelos metodos:
+switch (httpMethod) {
+case GET:
+	responses.addApiResponse("404", new ApiResponse().description("Recurso não encontrado"));
+	break;
+case POST:
+responses.addApiResponse("400", new ApiResponse().description("Requisição inválida"));
+…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26.13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Referenciando uma Respose</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Também podemos cira um mapa e fazer uma referência a ele:
+        apiResponseMap.put(internalServerErrorResponse, new ApiResponse()
+.description("Erro interno no servidor").content(content));
+…
+case DELETE:
+responses.addApiResponse("500", new ApiResponse().$ref(internalServerErrorResponse));
+ break;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26.16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Descrevendo Modelo do Problema</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Basta seguir o mesmo exemplo dos modelos e configurar no openApi Docs:
+@Schema(name = "Problema")
+public class Problem {…}
+Com isso teremos que registrar os schemas em openApi e depois referenciar em operations
+openApi...components(new Components().schemas(
+gerarSchemas()));
+@Operation(...@Content(schema = @Schema(ref = "Problema")))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26.14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Corrigindo Documentação com
+PageableParameter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Para representar parâmetros do tipo Pageable é necessário declarar vários parâmetros (page, size, sort)
+- Para melhorarmos a visibilidade e organização do código vamos criar uma anotação personalizada chamada PageableParameter
+- PageableParameter conterá todas as especificações e exemplos centralizados em uma única aotação:
+@Parameter(
+in = ParameterIn.QUERY,
+name = "sort",
+description = "Critério de ordenação: propriedade(asc|desc).",
+examples = { @ExampleObject("nome,desc") ...}
+)
+public @interface PageableParameter {...}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26.17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spring Authorizer Server</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'- Nova Solução Spring para Authorization Server segundo o padrão OAuth2.1
+- Novo projeto do Spring Framework que substitui o Spring Security Oauth que foi descontinuado
+- Spring Security Oauth foi dividido em dois projetos: Spring Security (Resource Server) e Spring Authorization Server
+- O spring authorization server já possui as dependencias do JWT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ajustando o Projecto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'- O AuthorizationServerConfig será completamente refatorado
+-  JwkSetController será removido
+- JwtCustomClaimsTokenEnhancer será reescrita
+- PkceAuthorizationCodeTokenGranter será removida
+- Security Controller será removido
+- Em ResourceServerConfig o WebSecurityConfigurerAdapter foi decpreciado e precisará ser refatorado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27.2</t>
   </si>
   <si>
     <t xml:space="preserve">ERRO</t>
@@ -4585,7 +5385,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -4616,10 +5416,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -4814,10 +5610,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F1048576"/>
+  <dimension ref="A1:F403"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A359" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B362" activeCellId="0" sqref="B362"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A394" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B396" activeCellId="0" sqref="B396"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5984,17 +6780,19 @@
       <c r="B106" s="6" t="s">
         <v>290</v>
       </c>
-      <c r="C106" s="4"/>
+      <c r="C106" s="4" t="s">
+        <v>291</v>
+      </c>
     </row>
     <row r="107" customFormat="false" ht="111" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A107" s="6" t="s">
+        <v>292</v>
+      </c>
+      <c r="B107" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="C107" s="4" t="s">
         <v>291</v>
-      </c>
-      <c r="B107" s="6" t="s">
-        <v>292</v>
-      </c>
-      <c r="C107" s="4" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="234.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6005,7 +6803,7 @@
         <v>295</v>
       </c>
       <c r="C108" s="4" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="150" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7732,1116 +8530,1492 @@
       <c r="B265" s="6" t="s">
         <v>734</v>
       </c>
-      <c r="C265" s="4"/>
+      <c r="C265" s="4" t="s">
+        <v>735</v>
+      </c>
     </row>
     <row r="266" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A266" s="6" t="s">
-        <v>735</v>
+        <v>736</v>
       </c>
       <c r="B266" s="6" t="s">
-        <v>736</v>
-      </c>
-      <c r="C266" s="4"/>
+        <v>737</v>
+      </c>
+      <c r="C266" s="4" t="s">
+        <v>738</v>
+      </c>
     </row>
     <row r="267" customFormat="false" ht="58.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A267" s="6" t="s">
-        <v>737</v>
+        <v>739</v>
       </c>
       <c r="B267" s="6" t="s">
+        <v>740</v>
+      </c>
+      <c r="C267" s="4" t="s">
         <v>738</v>
       </c>
-      <c r="C267" s="4"/>
     </row>
     <row r="268" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A268" s="6" t="s">
-        <v>739</v>
+        <v>741</v>
       </c>
       <c r="B268" s="6" t="s">
-        <v>740</v>
-      </c>
-      <c r="C268" s="4"/>
-    </row>
-    <row r="269" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>742</v>
+      </c>
+      <c r="C268" s="4" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="269" customFormat="false" ht="69.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A269" s="6" t="s">
-        <v>741</v>
+        <v>743</v>
       </c>
       <c r="B269" s="6" t="s">
-        <v>742</v>
-      </c>
-      <c r="C269" s="4"/>
+        <v>744</v>
+      </c>
+      <c r="C269" s="4" t="s">
+        <v>745</v>
+      </c>
     </row>
     <row r="270" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A270" s="6" t="s">
-        <v>743</v>
+        <v>746</v>
       </c>
       <c r="B270" s="6" t="s">
-        <v>744</v>
-      </c>
-      <c r="C270" s="4"/>
+        <v>747</v>
+      </c>
+      <c r="C270" s="4" t="s">
+        <v>745</v>
+      </c>
     </row>
     <row r="271" customFormat="false" ht="81.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A271" s="6" t="s">
-        <v>745</v>
+        <v>748</v>
       </c>
       <c r="B271" s="6" t="s">
-        <v>746</v>
-      </c>
-      <c r="C271" s="4"/>
-    </row>
-    <row r="272" customFormat="false" ht="92.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>749</v>
+      </c>
+      <c r="C271" s="4" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="272" customFormat="false" ht="113.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A272" s="6" t="s">
-        <v>747</v>
+        <v>751</v>
       </c>
       <c r="B272" s="6" t="s">
-        <v>748</v>
-      </c>
-      <c r="C272" s="4"/>
+        <v>752</v>
+      </c>
+      <c r="C272" s="4" t="s">
+        <v>753</v>
+      </c>
     </row>
     <row r="273" customFormat="false" ht="58.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A273" s="6" t="s">
-        <v>749</v>
+        <v>754</v>
       </c>
       <c r="B273" s="6" t="s">
-        <v>750</v>
-      </c>
-      <c r="C273" s="4"/>
-    </row>
-    <row r="274" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>755</v>
+      </c>
+      <c r="C273" s="4" t="s">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="274" customFormat="false" ht="95.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A274" s="6" t="s">
-        <v>751</v>
+        <v>756</v>
       </c>
       <c r="B274" s="6" t="s">
-        <v>752</v>
-      </c>
-      <c r="C274" s="4"/>
-    </row>
-    <row r="275" customFormat="false" ht="69.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>757</v>
+      </c>
+      <c r="C274" s="4" t="s">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="275" customFormat="false" ht="74.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A275" s="6" t="s">
-        <v>753</v>
+        <v>758</v>
       </c>
       <c r="B275" s="6" t="s">
-        <v>754</v>
-      </c>
-      <c r="C275" s="4"/>
-    </row>
-    <row r="276" customFormat="false" ht="58.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>759</v>
+      </c>
+      <c r="C275" s="4" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="276" customFormat="false" ht="60.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A276" s="6" t="s">
-        <v>755</v>
+        <v>761</v>
       </c>
       <c r="B276" s="6" t="s">
-        <v>756</v>
-      </c>
-      <c r="C276" s="4"/>
-    </row>
-    <row r="277" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>762</v>
+      </c>
+      <c r="C276" s="4" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="277" customFormat="false" ht="51.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A277" s="6" t="s">
-        <v>757</v>
+        <v>764</v>
       </c>
       <c r="B277" s="6" t="s">
-        <v>758</v>
-      </c>
-      <c r="C277" s="4"/>
-    </row>
-    <row r="278" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>765</v>
+      </c>
+      <c r="C277" s="4" t="s">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="278" customFormat="false" ht="167.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A278" s="6" t="s">
-        <v>759</v>
-      </c>
-      <c r="B278" s="6" t="s">
-        <v>760</v>
-      </c>
-      <c r="C278" s="4"/>
-    </row>
-    <row r="279" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>767</v>
+      </c>
+      <c r="B278" s="3" t="s">
+        <v>768</v>
+      </c>
+      <c r="C278" s="4" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="279" customFormat="false" ht="51.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A279" s="6" t="s">
-        <v>761</v>
+        <v>770</v>
       </c>
       <c r="B279" s="6" t="s">
-        <v>762</v>
-      </c>
-      <c r="C279" s="4"/>
-    </row>
-    <row r="280" customFormat="false" ht="81.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>771</v>
+      </c>
+      <c r="C279" s="4" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="280" customFormat="false" ht="35.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A280" s="6" t="s">
-        <v>763</v>
+        <v>772</v>
       </c>
       <c r="B280" s="6" t="s">
-        <v>764</v>
-      </c>
-      <c r="C280" s="4"/>
-    </row>
-    <row r="281" customFormat="false" ht="58.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>773</v>
+      </c>
+      <c r="C280" s="4" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="281" customFormat="false" ht="43.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A281" s="6" t="s">
-        <v>765</v>
+        <v>774</v>
       </c>
       <c r="B281" s="6" t="s">
-        <v>766</v>
-      </c>
-      <c r="C281" s="4"/>
-    </row>
-    <row r="282" customFormat="false" ht="92.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>775</v>
+      </c>
+      <c r="C281" s="4" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="282" customFormat="false" ht="86.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A282" s="6" t="s">
-        <v>767</v>
+        <v>777</v>
       </c>
       <c r="B282" s="6" t="s">
-        <v>768</v>
-      </c>
-      <c r="C282" s="4"/>
-    </row>
-    <row r="283" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>778</v>
+      </c>
+      <c r="C282" s="4" t="s">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="283" customFormat="false" ht="86.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A283" s="6" t="s">
-        <v>769</v>
+        <v>780</v>
       </c>
       <c r="B283" s="6" t="s">
-        <v>770</v>
-      </c>
-      <c r="C283" s="4"/>
-    </row>
-    <row r="284" customFormat="false" ht="253.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>781</v>
+      </c>
+      <c r="C283" s="4" t="s">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="284" customFormat="false" ht="74.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A284" s="6" t="s">
-        <v>771</v>
+        <v>783</v>
       </c>
       <c r="B284" s="6" t="s">
-        <v>772</v>
-      </c>
-      <c r="C284" s="4"/>
-    </row>
-    <row r="285" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>784</v>
+      </c>
+      <c r="C284" s="4" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="285" customFormat="false" ht="92.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A285" s="6" t="s">
-        <v>773</v>
+        <v>786</v>
       </c>
       <c r="B285" s="6" t="s">
-        <v>774</v>
-      </c>
-      <c r="C285" s="4"/>
-    </row>
-    <row r="286" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>787</v>
+      </c>
+      <c r="C285" s="4" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="286" customFormat="false" ht="65.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A286" s="6" t="s">
-        <v>775</v>
+        <v>789</v>
       </c>
       <c r="B286" s="6" t="s">
-        <v>776</v>
-      </c>
-      <c r="C286" s="4"/>
-    </row>
-    <row r="287" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>790</v>
+      </c>
+      <c r="C286" s="4" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="287" customFormat="false" ht="292.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A287" s="6" t="s">
-        <v>777</v>
+        <v>792</v>
       </c>
       <c r="B287" s="6" t="s">
-        <v>778</v>
-      </c>
-      <c r="C287" s="4"/>
-    </row>
-    <row r="288" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>793</v>
+      </c>
+      <c r="C287" s="4" t="s">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="288" customFormat="false" ht="39.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A288" s="6" t="s">
-        <v>779</v>
+        <v>795</v>
       </c>
       <c r="B288" s="6" t="s">
-        <v>780</v>
-      </c>
-      <c r="C288" s="4"/>
-    </row>
-    <row r="289" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>796</v>
+      </c>
+      <c r="C288" s="4" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="289" customFormat="false" ht="30.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A289" s="6" t="s">
-        <v>781</v>
+        <v>798</v>
       </c>
       <c r="B289" s="6" t="s">
-        <v>782</v>
-      </c>
-      <c r="C289" s="4"/>
-    </row>
-    <row r="290" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>799</v>
+      </c>
+      <c r="C289" s="4" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="290" customFormat="false" ht="54.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A290" s="6" t="s">
-        <v>783</v>
+        <v>800</v>
       </c>
       <c r="B290" s="6" t="s">
-        <v>784</v>
-      </c>
-      <c r="C290" s="4"/>
-    </row>
-    <row r="291" customFormat="false" ht="115.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>801</v>
+      </c>
+      <c r="C290" s="4" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="291" customFormat="false" ht="55.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A291" s="6" t="s">
-        <v>785</v>
+        <v>802</v>
       </c>
       <c r="B291" s="6" t="s">
-        <v>786</v>
-      </c>
-      <c r="C291" s="4"/>
-    </row>
-    <row r="292" customFormat="false" ht="162" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>803</v>
+      </c>
+      <c r="C291" s="4" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="292" customFormat="false" ht="109.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A292" s="6" t="s">
-        <v>787</v>
+        <v>805</v>
       </c>
       <c r="B292" s="6" t="s">
-        <v>788</v>
-      </c>
-      <c r="C292" s="4"/>
-    </row>
-    <row r="293" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>806</v>
+      </c>
+      <c r="C292" s="4" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="293" customFormat="false" ht="54.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A293" s="6" t="s">
-        <v>789</v>
+        <v>808</v>
       </c>
       <c r="B293" s="6" t="s">
-        <v>790</v>
-      </c>
-      <c r="C293" s="4"/>
-    </row>
-    <row r="294" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>809</v>
+      </c>
+      <c r="C293" s="4" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="294" customFormat="false" ht="42.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A294" s="6" t="s">
-        <v>791</v>
+        <v>811</v>
       </c>
       <c r="B294" s="6" t="s">
-        <v>792</v>
-      </c>
-      <c r="C294" s="4"/>
-    </row>
-    <row r="295" customFormat="false" ht="180.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>812</v>
+      </c>
+      <c r="C294" s="4" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="295" customFormat="false" ht="115.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A295" s="6" t="s">
-        <v>793</v>
+        <v>813</v>
       </c>
       <c r="B295" s="6" t="s">
-        <v>794</v>
-      </c>
-      <c r="C295" s="4"/>
-    </row>
-    <row r="296" customFormat="false" ht="127.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>814</v>
+      </c>
+      <c r="C295" s="4" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="296" customFormat="false" ht="50" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A296" s="6" t="s">
-        <v>795</v>
+        <v>815</v>
       </c>
       <c r="B296" s="6" t="s">
-        <v>796</v>
-      </c>
-      <c r="C296" s="4"/>
-    </row>
-    <row r="297" customFormat="false" ht="92.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>816</v>
+      </c>
+      <c r="C296" s="4" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="297" customFormat="false" ht="202.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A297" s="6" t="s">
-        <v>797</v>
+        <v>817</v>
       </c>
       <c r="B297" s="6" t="s">
-        <v>798</v>
-      </c>
-      <c r="C297" s="4"/>
-    </row>
-    <row r="298" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>818</v>
+      </c>
+      <c r="C297" s="4" t="s">
+        <v>819</v>
+      </c>
+    </row>
+    <row r="298" customFormat="false" ht="130.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A298" s="6" t="s">
-        <v>799</v>
+        <v>820</v>
       </c>
       <c r="B298" s="6" t="s">
-        <v>800</v>
-      </c>
-      <c r="C298" s="4"/>
-    </row>
-    <row r="299" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>821</v>
+      </c>
+      <c r="C298" s="4" t="s">
+        <v>822</v>
+      </c>
+    </row>
+    <row r="299" customFormat="false" ht="56.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A299" s="6" t="s">
-        <v>801</v>
+        <v>823</v>
       </c>
       <c r="B299" s="6" t="s">
-        <v>802</v>
-      </c>
-      <c r="C299" s="4"/>
-    </row>
-    <row r="300" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>824</v>
+      </c>
+      <c r="C299" s="4" t="s">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="300" customFormat="false" ht="156" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A300" s="6" t="s">
-        <v>803</v>
+        <v>826</v>
       </c>
       <c r="B300" s="6" t="s">
-        <v>804</v>
-      </c>
-      <c r="C300" s="4"/>
-    </row>
-    <row r="301" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>827</v>
+      </c>
+      <c r="C300" s="4" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="301" customFormat="false" ht="210.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A301" s="6" t="s">
-        <v>805</v>
+        <v>829</v>
       </c>
       <c r="B301" s="6" t="s">
-        <v>806</v>
-      </c>
-      <c r="C301" s="4"/>
-    </row>
-    <row r="302" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>830</v>
+      </c>
+      <c r="C301" s="4" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="302" customFormat="false" ht="200.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A302" s="6" t="s">
-        <v>807</v>
+        <v>832</v>
       </c>
       <c r="B302" s="6" t="s">
-        <v>808</v>
-      </c>
-      <c r="C302" s="4"/>
-    </row>
-    <row r="303" customFormat="false" ht="81.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>833</v>
+      </c>
+      <c r="C302" s="4" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="303" customFormat="false" ht="135.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A303" s="6" t="s">
-        <v>809</v>
+        <v>835</v>
       </c>
       <c r="B303" s="6" t="s">
-        <v>810</v>
-      </c>
-      <c r="C303" s="4"/>
-    </row>
-    <row r="304" customFormat="false" ht="58.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>836</v>
+      </c>
+      <c r="C303" s="4" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="304" customFormat="false" ht="92.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A304" s="6" t="s">
-        <v>811</v>
+        <v>837</v>
       </c>
       <c r="B304" s="6" t="s">
-        <v>812</v>
-      </c>
-      <c r="C304" s="4"/>
-    </row>
-    <row r="305" customFormat="false" ht="58.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>838</v>
+      </c>
+      <c r="C304" s="4" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="305" customFormat="false" ht="45.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A305" s="6" t="s">
-        <v>813</v>
+        <v>839</v>
       </c>
       <c r="B305" s="6" t="s">
-        <v>814</v>
-      </c>
-      <c r="C305" s="4"/>
-    </row>
-    <row r="306" customFormat="false" ht="69.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>840</v>
+      </c>
+      <c r="C305" s="4" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="306" customFormat="false" ht="79.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A306" s="6" t="s">
-        <v>815</v>
+        <v>841</v>
       </c>
       <c r="B306" s="6" t="s">
-        <v>816</v>
-      </c>
-      <c r="C306" s="4"/>
-    </row>
-    <row r="307" customFormat="false" ht="104.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>842</v>
+      </c>
+      <c r="C306" s="4" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="307" customFormat="false" ht="180.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A307" s="6" t="s">
-        <v>817</v>
+        <v>844</v>
       </c>
       <c r="B307" s="6" t="s">
-        <v>818</v>
-      </c>
-      <c r="C307" s="4"/>
-    </row>
-    <row r="308" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>845</v>
+      </c>
+      <c r="C307" s="4" t="s">
+        <v>846</v>
+      </c>
+    </row>
+    <row r="308" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A308" s="6" t="s">
-        <v>819</v>
+        <v>847</v>
       </c>
       <c r="B308" s="6" t="s">
-        <v>820</v>
-      </c>
-      <c r="C308" s="4"/>
+        <v>848</v>
+      </c>
+      <c r="C308" s="4" t="s">
+        <v>849</v>
+      </c>
     </row>
     <row r="309" customFormat="false" ht="104.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A309" s="6" t="s">
-        <v>821</v>
+        <v>850</v>
       </c>
       <c r="B309" s="6" t="s">
-        <v>822</v>
-      </c>
-      <c r="C309" s="4"/>
-    </row>
-    <row r="310" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>851</v>
+      </c>
+      <c r="C309" s="4" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="310" customFormat="false" ht="124.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A310" s="6" t="s">
-        <v>823</v>
+        <v>852</v>
       </c>
       <c r="B310" s="6" t="s">
-        <v>824</v>
-      </c>
-      <c r="C310" s="4"/>
-    </row>
-    <row r="311" customFormat="false" ht="69.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>853</v>
+      </c>
+      <c r="C310" s="4" t="s">
+        <v>854</v>
+      </c>
+    </row>
+    <row r="311" customFormat="false" ht="112.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A311" s="6" t="s">
-        <v>825</v>
+        <v>855</v>
       </c>
       <c r="B311" s="6" t="s">
-        <v>826</v>
-      </c>
-      <c r="C311" s="4"/>
-    </row>
-    <row r="312" customFormat="false" ht="106.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>856</v>
+      </c>
+      <c r="C311" s="4" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="312" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A312" s="6" t="s">
-        <v>827</v>
+        <v>858</v>
       </c>
       <c r="B312" s="6" t="s">
-        <v>828</v>
-      </c>
-      <c r="C312" s="4"/>
-    </row>
-    <row r="313" customFormat="false" ht="46.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>859</v>
+      </c>
+      <c r="C312" s="4" t="s">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="313" customFormat="false" ht="81.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A313" s="6" t="s">
-        <v>829</v>
+        <v>861</v>
       </c>
       <c r="B313" s="6" t="s">
-        <v>830</v>
+        <v>862</v>
       </c>
       <c r="C313" s="4" t="s">
-        <v>831</v>
-      </c>
-    </row>
-    <row r="314" customFormat="false" ht="138" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="314" customFormat="false" ht="257.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A314" s="6" t="s">
-        <v>832</v>
+        <v>864</v>
       </c>
       <c r="B314" s="6" t="s">
-        <v>833</v>
+        <v>865</v>
       </c>
       <c r="C314" s="4" t="s">
-        <v>834</v>
-      </c>
-    </row>
-    <row r="315" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="315" customFormat="false" ht="69.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A315" s="6" t="s">
-        <v>835</v>
+        <v>867</v>
       </c>
       <c r="B315" s="6" t="s">
-        <v>836</v>
+        <v>868</v>
       </c>
       <c r="C315" s="4" t="s">
-        <v>837</v>
-      </c>
-    </row>
-    <row r="316" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="316" customFormat="false" ht="106.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A316" s="6" t="s">
-        <v>838</v>
+        <v>870</v>
       </c>
       <c r="B316" s="6" t="s">
-        <v>839</v>
+        <v>871</v>
       </c>
       <c r="C316" s="4" t="s">
-        <v>837</v>
-      </c>
-    </row>
-    <row r="317" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>872</v>
+      </c>
+    </row>
+    <row r="317" customFormat="false" ht="118.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A317" s="6" t="s">
-        <v>840</v>
+        <v>873</v>
       </c>
       <c r="B317" s="6" t="s">
-        <v>841</v>
+        <v>874</v>
       </c>
       <c r="C317" s="4" t="s">
-        <v>837</v>
-      </c>
-    </row>
-    <row r="318" customFormat="false" ht="69" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="318" customFormat="false" ht="104.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A318" s="6" t="s">
-        <v>842</v>
+        <v>876</v>
       </c>
       <c r="B318" s="6" t="s">
-        <v>843</v>
+        <v>877</v>
       </c>
       <c r="C318" s="4" t="s">
-        <v>844</v>
-      </c>
-    </row>
-    <row r="319" customFormat="false" ht="46.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="319" customFormat="false" ht="77.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A319" s="6" t="s">
-        <v>845</v>
+        <v>879</v>
       </c>
       <c r="B319" s="6" t="s">
-        <v>846</v>
+        <v>880</v>
       </c>
       <c r="C319" s="4" t="s">
-        <v>847</v>
-      </c>
-    </row>
-    <row r="320" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="320" customFormat="false" ht="43.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A320" s="6" t="s">
-        <v>848</v>
+        <v>882</v>
       </c>
       <c r="B320" s="6" t="s">
-        <v>849</v>
+        <v>883</v>
       </c>
       <c r="C320" s="4" t="s">
-        <v>847</v>
-      </c>
-    </row>
-    <row r="321" customFormat="false" ht="144" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>884</v>
+      </c>
+    </row>
+    <row r="321" customFormat="false" ht="207.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A321" s="6" t="s">
-        <v>850</v>
+        <v>885</v>
       </c>
       <c r="B321" s="6" t="s">
-        <v>851</v>
+        <v>886</v>
       </c>
       <c r="C321" s="4" t="s">
-        <v>852</v>
-      </c>
-    </row>
-    <row r="322" customFormat="false" ht="142.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>887</v>
+      </c>
+    </row>
+    <row r="322" customFormat="false" ht="78.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A322" s="6" t="s">
-        <v>853</v>
+        <v>888</v>
       </c>
       <c r="B322" s="6" t="s">
-        <v>854</v>
+        <v>889</v>
       </c>
       <c r="C322" s="4" t="s">
-        <v>855</v>
-      </c>
-    </row>
-    <row r="323" customFormat="false" ht="42" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="323" customFormat="false" ht="45.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A323" s="6" t="s">
-        <v>856</v>
+        <v>891</v>
       </c>
       <c r="B323" s="6" t="s">
-        <v>857</v>
+        <v>892</v>
       </c>
       <c r="C323" s="4" t="s">
-        <v>858</v>
-      </c>
-    </row>
-    <row r="324" customFormat="false" ht="82.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>893</v>
+      </c>
+    </row>
+    <row r="324" customFormat="false" ht="108.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A324" s="6" t="s">
-        <v>859</v>
+        <v>894</v>
       </c>
       <c r="B324" s="6" t="s">
-        <v>860</v>
+        <v>895</v>
       </c>
       <c r="C324" s="4" t="s">
-        <v>861</v>
-      </c>
-    </row>
-    <row r="325" customFormat="false" ht="74.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>893</v>
+      </c>
+    </row>
+    <row r="325" customFormat="false" ht="178.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A325" s="6" t="s">
-        <v>862</v>
+        <v>896</v>
       </c>
       <c r="B325" s="6" t="s">
-        <v>863</v>
+        <v>897</v>
       </c>
       <c r="C325" s="4" t="s">
-        <v>864</v>
-      </c>
-    </row>
-    <row r="326" customFormat="false" ht="110.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>893</v>
+      </c>
+    </row>
+    <row r="326" customFormat="false" ht="228.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A326" s="6" t="s">
-        <v>865</v>
+        <v>898</v>
       </c>
       <c r="B326" s="6" t="s">
-        <v>866</v>
+        <v>899</v>
       </c>
       <c r="C326" s="4" t="s">
-        <v>867</v>
-      </c>
-    </row>
-    <row r="327" customFormat="false" ht="234.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="327" customFormat="false" ht="46.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A327" s="6" t="s">
-        <v>868</v>
+        <v>901</v>
       </c>
       <c r="B327" s="6" t="s">
-        <v>869</v>
+        <v>902</v>
       </c>
       <c r="C327" s="4" t="s">
-        <v>870</v>
-      </c>
-    </row>
-    <row r="328" customFormat="false" ht="138.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>903</v>
+      </c>
+    </row>
+    <row r="328" customFormat="false" ht="138" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A328" s="6" t="s">
-        <v>871</v>
+        <v>904</v>
       </c>
       <c r="B328" s="6" t="s">
-        <v>872</v>
+        <v>905</v>
       </c>
       <c r="C328" s="4" t="s">
-        <v>870</v>
-      </c>
-    </row>
-    <row r="329" customFormat="false" ht="99" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>906</v>
+      </c>
+    </row>
+    <row r="329" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A329" s="6" t="s">
-        <v>873</v>
+        <v>907</v>
       </c>
       <c r="B329" s="6" t="s">
-        <v>874</v>
+        <v>908</v>
       </c>
       <c r="C329" s="4" t="s">
-        <v>870</v>
-      </c>
-    </row>
-    <row r="330" customFormat="false" ht="48" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>909</v>
+      </c>
+    </row>
+    <row r="330" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A330" s="6" t="s">
-        <v>875</v>
+        <v>910</v>
       </c>
       <c r="B330" s="6" t="s">
-        <v>876</v>
+        <v>911</v>
       </c>
       <c r="C330" s="4" t="s">
-        <v>877</v>
-      </c>
-    </row>
-    <row r="331" customFormat="false" ht="47.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>909</v>
+      </c>
+    </row>
+    <row r="331" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A331" s="6" t="s">
-        <v>878</v>
+        <v>912</v>
       </c>
       <c r="B331" s="6" t="s">
-        <v>879</v>
+        <v>913</v>
       </c>
       <c r="C331" s="4" t="s">
-        <v>880</v>
-      </c>
-    </row>
-    <row r="332" customFormat="false" ht="224.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>909</v>
+      </c>
+    </row>
+    <row r="332" customFormat="false" ht="69" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A332" s="6" t="s">
-        <v>881</v>
+        <v>914</v>
       </c>
       <c r="B332" s="6" t="s">
-        <v>882</v>
+        <v>915</v>
       </c>
       <c r="C332" s="4" t="s">
-        <v>880</v>
-      </c>
-    </row>
-    <row r="333" customFormat="false" ht="88.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="333" customFormat="false" ht="46.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A333" s="6" t="s">
-        <v>883</v>
+        <v>917</v>
       </c>
       <c r="B333" s="6" t="s">
-        <v>884</v>
+        <v>918</v>
       </c>
       <c r="C333" s="4" t="s">
-        <v>885</v>
-      </c>
-    </row>
-    <row r="334" customFormat="false" ht="228.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>919</v>
+      </c>
+    </row>
+    <row r="334" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A334" s="6" t="s">
-        <v>886</v>
+        <v>920</v>
       </c>
       <c r="B334" s="6" t="s">
-        <v>887</v>
+        <v>921</v>
       </c>
       <c r="C334" s="4" t="s">
-        <v>888</v>
-      </c>
-    </row>
-    <row r="335" customFormat="false" ht="125.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>919</v>
+      </c>
+    </row>
+    <row r="335" customFormat="false" ht="144" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A335" s="6" t="s">
-        <v>889</v>
+        <v>922</v>
       </c>
       <c r="B335" s="6" t="s">
-        <v>890</v>
+        <v>923</v>
       </c>
       <c r="C335" s="4" t="s">
-        <v>891</v>
-      </c>
-    </row>
-    <row r="336" customFormat="false" ht="93.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>924</v>
+      </c>
+    </row>
+    <row r="336" customFormat="false" ht="142.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A336" s="6" t="s">
-        <v>892</v>
+        <v>925</v>
       </c>
       <c r="B336" s="6" t="s">
-        <v>893</v>
+        <v>926</v>
       </c>
       <c r="C336" s="4" t="s">
-        <v>894</v>
-      </c>
-    </row>
-    <row r="337" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>927</v>
+      </c>
+    </row>
+    <row r="337" customFormat="false" ht="42" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A337" s="6" t="s">
-        <v>895</v>
+        <v>928</v>
       </c>
       <c r="B337" s="6" t="s">
-        <v>896</v>
+        <v>929</v>
       </c>
       <c r="C337" s="4" t="s">
-        <v>897</v>
-      </c>
-    </row>
-    <row r="338" customFormat="false" ht="55.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>930</v>
+      </c>
+    </row>
+    <row r="338" customFormat="false" ht="82.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A338" s="6" t="s">
-        <v>898</v>
+        <v>931</v>
       </c>
       <c r="B338" s="6" t="s">
-        <v>899</v>
+        <v>932</v>
       </c>
       <c r="C338" s="4" t="s">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="339" customFormat="false" ht="56.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="339" customFormat="false" ht="74.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A339" s="6" t="s">
-        <v>901</v>
+        <v>934</v>
       </c>
       <c r="B339" s="6" t="s">
-        <v>902</v>
+        <v>935</v>
       </c>
       <c r="C339" s="4" t="s">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="340" customFormat="false" ht="60" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="340" customFormat="false" ht="110.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A340" s="6" t="s">
-        <v>903</v>
+        <v>937</v>
       </c>
       <c r="B340" s="6" t="s">
-        <v>904</v>
+        <v>938</v>
       </c>
       <c r="C340" s="4" t="s">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="341" customFormat="false" ht="135" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="341" customFormat="false" ht="234.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A341" s="6" t="s">
-        <v>905</v>
+        <v>940</v>
       </c>
       <c r="B341" s="6" t="s">
-        <v>906</v>
+        <v>941</v>
       </c>
       <c r="C341" s="4" t="s">
-        <v>907</v>
-      </c>
-    </row>
-    <row r="342" customFormat="false" ht="85.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>942</v>
+      </c>
+    </row>
+    <row r="342" customFormat="false" ht="138.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A342" s="6" t="s">
-        <v>908</v>
+        <v>943</v>
       </c>
       <c r="B342" s="6" t="s">
-        <v>909</v>
+        <v>944</v>
       </c>
       <c r="C342" s="4" t="s">
-        <v>910</v>
-      </c>
-    </row>
-    <row r="343" customFormat="false" ht="118.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>942</v>
+      </c>
+    </row>
+    <row r="343" customFormat="false" ht="99" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A343" s="6" t="s">
-        <v>911</v>
+        <v>945</v>
       </c>
       <c r="B343" s="6" t="s">
-        <v>912</v>
+        <v>946</v>
       </c>
       <c r="C343" s="4" t="s">
-        <v>913</v>
-      </c>
-    </row>
-    <row r="344" customFormat="false" ht="120" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>942</v>
+      </c>
+    </row>
+    <row r="344" customFormat="false" ht="48" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A344" s="6" t="s">
-        <v>914</v>
+        <v>947</v>
       </c>
       <c r="B344" s="6" t="s">
-        <v>915</v>
+        <v>948</v>
       </c>
       <c r="C344" s="4" t="s">
-        <v>916</v>
-      </c>
-    </row>
-    <row r="345" customFormat="false" ht="53.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>949</v>
+      </c>
+    </row>
+    <row r="345" customFormat="false" ht="47.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A345" s="6" t="s">
-        <v>917</v>
+        <v>950</v>
       </c>
       <c r="B345" s="6" t="s">
-        <v>918</v>
+        <v>951</v>
       </c>
       <c r="C345" s="4" t="s">
-        <v>919</v>
-      </c>
-    </row>
-    <row r="346" customFormat="false" ht="81" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>952</v>
+      </c>
+    </row>
+    <row r="346" customFormat="false" ht="224.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A346" s="6" t="s">
-        <v>920</v>
+        <v>953</v>
       </c>
       <c r="B346" s="6" t="s">
-        <v>921</v>
+        <v>954</v>
       </c>
       <c r="C346" s="4" t="s">
-        <v>919</v>
-      </c>
-    </row>
-    <row r="347" customFormat="false" ht="119.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>952</v>
+      </c>
+    </row>
+    <row r="347" customFormat="false" ht="88.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A347" s="6" t="s">
-        <v>922</v>
+        <v>955</v>
       </c>
       <c r="B347" s="6" t="s">
-        <v>923</v>
+        <v>956</v>
       </c>
       <c r="C347" s="4" t="s">
-        <v>919</v>
-      </c>
-    </row>
-    <row r="348" customFormat="false" ht="198" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>957</v>
+      </c>
+    </row>
+    <row r="348" customFormat="false" ht="228.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A348" s="6" t="s">
-        <v>924</v>
+        <v>958</v>
       </c>
       <c r="B348" s="6" t="s">
-        <v>925</v>
+        <v>959</v>
       </c>
       <c r="C348" s="4" t="s">
-        <v>926</v>
-      </c>
-    </row>
-    <row r="349" customFormat="false" ht="87" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="349" customFormat="false" ht="125.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A349" s="6" t="s">
-        <v>927</v>
+        <v>961</v>
       </c>
       <c r="B349" s="6" t="s">
-        <v>928</v>
+        <v>962</v>
       </c>
       <c r="C349" s="4" t="s">
-        <v>929</v>
-      </c>
-    </row>
-    <row r="350" customFormat="false" ht="156.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>963</v>
+      </c>
+    </row>
+    <row r="350" customFormat="false" ht="93.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A350" s="6" t="s">
-        <v>930</v>
+        <v>964</v>
       </c>
       <c r="B350" s="6" t="s">
-        <v>931</v>
+        <v>965</v>
       </c>
       <c r="C350" s="4" t="s">
-        <v>932</v>
-      </c>
-    </row>
-    <row r="351" customFormat="false" ht="105" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="351" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A351" s="6" t="s">
-        <v>933</v>
+        <v>967</v>
       </c>
       <c r="B351" s="6" t="s">
-        <v>934</v>
+        <v>968</v>
       </c>
       <c r="C351" s="4" t="s">
-        <v>935</v>
-      </c>
-    </row>
-    <row r="352" customFormat="false" ht="79.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>969</v>
+      </c>
+    </row>
+    <row r="352" customFormat="false" ht="55.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A352" s="6" t="s">
-        <v>936</v>
+        <v>970</v>
       </c>
       <c r="B352" s="6" t="s">
-        <v>937</v>
+        <v>971</v>
       </c>
       <c r="C352" s="4" t="s">
-        <v>938</v>
-      </c>
-    </row>
-    <row r="353" customFormat="false" ht="92.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>972</v>
+      </c>
+    </row>
+    <row r="353" customFormat="false" ht="56.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A353" s="6" t="s">
-        <v>939</v>
+        <v>973</v>
       </c>
       <c r="B353" s="6" t="s">
-        <v>940</v>
+        <v>974</v>
       </c>
       <c r="C353" s="4" t="s">
-        <v>941</v>
-      </c>
-    </row>
-    <row r="354" customFormat="false" ht="78" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>972</v>
+      </c>
+    </row>
+    <row r="354" customFormat="false" ht="60" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A354" s="6" t="s">
-        <v>942</v>
+        <v>975</v>
       </c>
       <c r="B354" s="6" t="s">
-        <v>943</v>
+        <v>976</v>
       </c>
       <c r="C354" s="4" t="s">
-        <v>944</v>
-      </c>
-    </row>
-    <row r="355" customFormat="false" ht="55.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>972</v>
+      </c>
+    </row>
+    <row r="355" customFormat="false" ht="135" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A355" s="6" t="s">
-        <v>945</v>
+        <v>977</v>
       </c>
       <c r="B355" s="6" t="s">
-        <v>946</v>
+        <v>978</v>
       </c>
       <c r="C355" s="4" t="s">
-        <v>944</v>
-      </c>
-    </row>
-    <row r="356" customFormat="false" ht="69.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="356" customFormat="false" ht="85.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A356" s="6" t="s">
-        <v>947</v>
+        <v>980</v>
       </c>
       <c r="B356" s="6" t="s">
-        <v>948</v>
+        <v>981</v>
       </c>
       <c r="C356" s="4" t="s">
-        <v>949</v>
-      </c>
-    </row>
-    <row r="357" customFormat="false" ht="108.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>982</v>
+      </c>
+    </row>
+    <row r="357" customFormat="false" ht="118.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A357" s="6" t="s">
-        <v>950</v>
+        <v>983</v>
       </c>
       <c r="B357" s="6" t="s">
-        <v>951</v>
+        <v>984</v>
       </c>
       <c r="C357" s="4" t="s">
-        <v>949</v>
-      </c>
-    </row>
-    <row r="358" customFormat="false" ht="74.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>985</v>
+      </c>
+    </row>
+    <row r="358" customFormat="false" ht="120" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A358" s="6" t="s">
-        <v>952</v>
+        <v>986</v>
       </c>
       <c r="B358" s="6" t="s">
-        <v>953</v>
+        <v>987</v>
       </c>
       <c r="C358" s="4" t="s">
-        <v>954</v>
-      </c>
-    </row>
-    <row r="359" customFormat="false" ht="106.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>988</v>
+      </c>
+    </row>
+    <row r="359" customFormat="false" ht="53.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A359" s="6" t="s">
-        <v>955</v>
+        <v>989</v>
       </c>
       <c r="B359" s="6" t="s">
-        <v>956</v>
+        <v>990</v>
       </c>
       <c r="C359" s="4" t="s">
-        <v>954</v>
-      </c>
-    </row>
-    <row r="360" customFormat="false" ht="179.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>991</v>
+      </c>
+    </row>
+    <row r="360" customFormat="false" ht="81" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A360" s="6" t="s">
-        <v>957</v>
+        <v>992</v>
       </c>
       <c r="B360" s="6" t="s">
-        <v>958</v>
+        <v>993</v>
       </c>
       <c r="C360" s="4" t="s">
-        <v>959</v>
-      </c>
-    </row>
-    <row r="361" customFormat="false" ht="59" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>991</v>
+      </c>
+    </row>
+    <row r="361" customFormat="false" ht="119.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A361" s="6" t="s">
-        <v>960</v>
+        <v>994</v>
       </c>
       <c r="B361" s="6" t="s">
-        <v>961</v>
-      </c>
-      <c r="C361" s="8" t="s">
-        <v>962</v>
-      </c>
-    </row>
-    <row r="362" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A362" s="6"/>
-      <c r="B362" s="6"/>
-      <c r="C362" s="6"/>
-    </row>
-    <row r="363" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A363" s="6"/>
-      <c r="B363" s="6"/>
-      <c r="C363" s="6"/>
-    </row>
-    <row r="364" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A364" s="6"/>
-      <c r="B364" s="6"/>
-      <c r="C364" s="6"/>
-    </row>
-    <row r="365" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A365" s="6"/>
-      <c r="B365" s="6"/>
-      <c r="C365" s="6"/>
-    </row>
-    <row r="366" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A366" s="6"/>
-      <c r="B366" s="6"/>
-      <c r="C366" s="6"/>
-    </row>
-    <row r="367" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A367" s="6"/>
-      <c r="B367" s="6"/>
-      <c r="C367" s="6"/>
-    </row>
-    <row r="368" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A368" s="6"/>
-      <c r="B368" s="6"/>
-      <c r="C368" s="6"/>
-    </row>
-    <row r="369" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A369" s="6"/>
-      <c r="B369" s="6"/>
-      <c r="C369" s="6"/>
-    </row>
-    <row r="370" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A370" s="6"/>
-      <c r="B370" s="6"/>
-      <c r="C370" s="6"/>
-    </row>
-    <row r="371" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A371" s="6"/>
-      <c r="B371" s="6"/>
-      <c r="C371" s="6"/>
-    </row>
-    <row r="372" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A372" s="6"/>
-      <c r="B372" s="6"/>
-      <c r="C372" s="6"/>
-    </row>
-    <row r="373" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A373" s="6"/>
-      <c r="B373" s="6"/>
-      <c r="C373" s="6"/>
-    </row>
-    <row r="374" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A374" s="6"/>
-      <c r="B374" s="6"/>
-      <c r="C374" s="6"/>
-    </row>
-    <row r="375" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A375" s="6"/>
-      <c r="B375" s="6"/>
-      <c r="C375" s="6"/>
+        <v>995</v>
+      </c>
+      <c r="C361" s="4" t="s">
+        <v>991</v>
+      </c>
+    </row>
+    <row r="362" customFormat="false" ht="198" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A362" s="6" t="s">
+        <v>996</v>
+      </c>
+      <c r="B362" s="6" t="s">
+        <v>997</v>
+      </c>
+      <c r="C362" s="4" t="s">
+        <v>998</v>
+      </c>
+    </row>
+    <row r="363" customFormat="false" ht="87" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A363" s="6" t="s">
+        <v>999</v>
+      </c>
+      <c r="B363" s="6" t="s">
+        <v>1000</v>
+      </c>
+      <c r="C363" s="4" t="s">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="364" customFormat="false" ht="156.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A364" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="B364" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="C364" s="4" t="s">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="365" customFormat="false" ht="105" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A365" s="6" t="s">
+        <v>1005</v>
+      </c>
+      <c r="B365" s="6" t="s">
+        <v>1006</v>
+      </c>
+      <c r="C365" s="4" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="366" customFormat="false" ht="79.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A366" s="6" t="s">
+        <v>1008</v>
+      </c>
+      <c r="B366" s="6" t="s">
+        <v>1009</v>
+      </c>
+      <c r="C366" s="4" t="s">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="367" customFormat="false" ht="92.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A367" s="6" t="s">
+        <v>1011</v>
+      </c>
+      <c r="B367" s="6" t="s">
+        <v>1012</v>
+      </c>
+      <c r="C367" s="4" t="s">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="368" customFormat="false" ht="78" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A368" s="6" t="s">
+        <v>1014</v>
+      </c>
+      <c r="B368" s="6" t="s">
+        <v>1015</v>
+      </c>
+      <c r="C368" s="4" t="s">
+        <v>1016</v>
+      </c>
+    </row>
+    <row r="369" customFormat="false" ht="55.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A369" s="6" t="s">
+        <v>1017</v>
+      </c>
+      <c r="B369" s="6" t="s">
+        <v>1018</v>
+      </c>
+      <c r="C369" s="4" t="s">
+        <v>1016</v>
+      </c>
+    </row>
+    <row r="370" customFormat="false" ht="69.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A370" s="6" t="s">
+        <v>1019</v>
+      </c>
+      <c r="B370" s="6" t="s">
+        <v>1020</v>
+      </c>
+      <c r="C370" s="4" t="s">
+        <v>1021</v>
+      </c>
+    </row>
+    <row r="371" customFormat="false" ht="108.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A371" s="6" t="s">
+        <v>1022</v>
+      </c>
+      <c r="B371" s="6" t="s">
+        <v>1023</v>
+      </c>
+      <c r="C371" s="4" t="s">
+        <v>1021</v>
+      </c>
+    </row>
+    <row r="372" customFormat="false" ht="74.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A372" s="6" t="s">
+        <v>1024</v>
+      </c>
+      <c r="B372" s="6" t="s">
+        <v>1025</v>
+      </c>
+      <c r="C372" s="4" t="s">
+        <v>1026</v>
+      </c>
+    </row>
+    <row r="373" customFormat="false" ht="106.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A373" s="6" t="s">
+        <v>1027</v>
+      </c>
+      <c r="B373" s="6" t="s">
+        <v>1028</v>
+      </c>
+      <c r="C373" s="4" t="s">
+        <v>1026</v>
+      </c>
+    </row>
+    <row r="374" customFormat="false" ht="179.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A374" s="6" t="s">
+        <v>1029</v>
+      </c>
+      <c r="B374" s="6" t="s">
+        <v>1030</v>
+      </c>
+      <c r="C374" s="4" t="s">
+        <v>1031</v>
+      </c>
+    </row>
+    <row r="375" customFormat="false" ht="59" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A375" s="6" t="s">
+        <v>1032</v>
+      </c>
+      <c r="B375" s="6" t="s">
+        <v>1033</v>
+      </c>
+      <c r="C375" s="6" t="s">
+        <v>1034</v>
+      </c>
     </row>
     <row r="376" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A376" s="6"/>
-      <c r="B376" s="6"/>
-      <c r="C376" s="6"/>
-    </row>
-    <row r="377" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A377" s="6"/>
-      <c r="B377" s="6"/>
-      <c r="C377" s="6"/>
-    </row>
-    <row r="378" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A378" s="6"/>
-      <c r="B378" s="6"/>
-      <c r="C378" s="6"/>
-    </row>
-    <row r="379" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A379" s="6"/>
-      <c r="B379" s="6"/>
-      <c r="C379" s="6"/>
-    </row>
-    <row r="380" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A380" s="6"/>
-      <c r="B380" s="6"/>
-      <c r="C380" s="6"/>
-    </row>
-    <row r="381" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A381" s="6"/>
-      <c r="B381" s="6"/>
-      <c r="C381" s="6"/>
-    </row>
-    <row r="382" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A382" s="6"/>
-      <c r="B382" s="6"/>
-      <c r="C382" s="6"/>
-    </row>
-    <row r="383" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A383" s="6"/>
-      <c r="B383" s="6"/>
-      <c r="C383" s="6"/>
-    </row>
-    <row r="384" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A384" s="6"/>
-      <c r="B384" s="6"/>
-      <c r="C384" s="6"/>
-    </row>
-    <row r="385" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A385" s="6"/>
-      <c r="B385" s="6"/>
-      <c r="C385" s="6"/>
-    </row>
-    <row r="386" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A386" s="6"/>
-      <c r="B386" s="6"/>
-      <c r="C386" s="6"/>
-    </row>
-    <row r="387" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A387" s="6"/>
-      <c r="B387" s="6"/>
-      <c r="C387" s="6"/>
-    </row>
-    <row r="388" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A388" s="6"/>
-      <c r="B388" s="6"/>
-      <c r="C388" s="6"/>
-    </row>
-    <row r="389" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A389" s="6"/>
-      <c r="B389" s="6"/>
-      <c r="C389" s="6"/>
-    </row>
-    <row r="390" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A390" s="6"/>
-      <c r="B390" s="6"/>
-      <c r="C390" s="6"/>
-    </row>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="A376" s="6" t="s">
+        <v>1035</v>
+      </c>
+      <c r="B376" s="6" t="s">
+        <v>1036</v>
+      </c>
+      <c r="C376" s="6" t="s">
+        <v>1037</v>
+      </c>
+    </row>
+    <row r="377" customFormat="false" ht="61.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A377" s="6" t="s">
+        <v>1038</v>
+      </c>
+      <c r="B377" s="6" t="s">
+        <v>1039</v>
+      </c>
+      <c r="C377" s="6" t="s">
+        <v>1040</v>
+      </c>
+    </row>
+    <row r="378" customFormat="false" ht="69.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A378" s="6" t="s">
+        <v>1041</v>
+      </c>
+      <c r="B378" s="6" t="s">
+        <v>1042</v>
+      </c>
+      <c r="C378" s="6" t="s">
+        <v>1040</v>
+      </c>
+    </row>
+    <row r="379" customFormat="false" ht="79.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A379" s="6" t="s">
+        <v>1043</v>
+      </c>
+      <c r="B379" s="6" t="s">
+        <v>1044</v>
+      </c>
+      <c r="C379" s="6" t="s">
+        <v>1040</v>
+      </c>
+    </row>
+    <row r="380" customFormat="false" ht="121.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A380" s="6" t="s">
+        <v>1045</v>
+      </c>
+      <c r="B380" s="6" t="s">
+        <v>1046</v>
+      </c>
+      <c r="C380" s="6" t="s">
+        <v>1047</v>
+      </c>
+    </row>
+    <row r="381" customFormat="false" ht="242.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A381" s="6" t="s">
+        <v>1048</v>
+      </c>
+      <c r="B381" s="6" t="s">
+        <v>1049</v>
+      </c>
+      <c r="C381" s="6" t="s">
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="382" customFormat="false" ht="121.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A382" s="6" t="s">
+        <v>1051</v>
+      </c>
+      <c r="B382" s="6" t="s">
+        <v>1052</v>
+      </c>
+      <c r="C382" s="6" t="s">
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="383" customFormat="false" ht="40.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A383" s="6" t="s">
+        <v>1053</v>
+      </c>
+      <c r="B383" s="6" t="s">
+        <v>1054</v>
+      </c>
+      <c r="C383" s="6" t="s">
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="384" customFormat="false" ht="41.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A384" s="6" t="s">
+        <v>1055</v>
+      </c>
+      <c r="B384" s="6" t="s">
+        <v>1056</v>
+      </c>
+      <c r="C384" s="6" t="s">
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="385" customFormat="false" ht="43.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A385" s="6" t="s">
+        <v>1057</v>
+      </c>
+      <c r="B385" s="6" t="s">
+        <v>1058</v>
+      </c>
+      <c r="C385" s="6" t="s">
+        <v>1059</v>
+      </c>
+    </row>
+    <row r="386" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A386" s="6" t="s">
+        <v>1060</v>
+      </c>
+      <c r="B386" s="6" t="s">
+        <v>1061</v>
+      </c>
+      <c r="C386" s="6" t="s">
+        <v>1062</v>
+      </c>
+    </row>
+    <row r="387" customFormat="false" ht="70.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A387" s="6" t="s">
+        <v>1063</v>
+      </c>
+      <c r="B387" s="6" t="s">
+        <v>1064</v>
+      </c>
+      <c r="C387" s="6" t="s">
+        <v>1065</v>
+      </c>
+    </row>
+    <row r="388" customFormat="false" ht="74.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A388" s="6" t="s">
+        <v>1066</v>
+      </c>
+      <c r="B388" s="6" t="s">
+        <v>1067</v>
+      </c>
+      <c r="C388" s="6" t="s">
+        <v>1068</v>
+      </c>
+    </row>
+    <row r="389" customFormat="false" ht="75.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A389" s="6" t="s">
+        <v>1069</v>
+      </c>
+      <c r="B389" s="6" t="s">
+        <v>1070</v>
+      </c>
+      <c r="C389" s="6" t="s">
+        <v>1071</v>
+      </c>
+    </row>
+    <row r="390" customFormat="false" ht="54.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A390" s="6" t="s">
+        <v>1072</v>
+      </c>
+      <c r="B390" s="6" t="s">
+        <v>1073</v>
+      </c>
+      <c r="C390" s="6" t="s">
+        <v>1074</v>
+      </c>
+    </row>
+    <row r="391" customFormat="false" ht="89.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A391" s="6" t="s">
+        <v>1075</v>
+      </c>
+      <c r="B391" s="6" t="s">
+        <v>1076</v>
+      </c>
+      <c r="C391" s="6" t="s">
+        <v>1077</v>
+      </c>
+    </row>
+    <row r="392" customFormat="false" ht="119.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A392" s="6" t="s">
+        <v>1078</v>
+      </c>
+      <c r="B392" s="6" t="s">
+        <v>1079</v>
+      </c>
+      <c r="C392" s="6" t="s">
+        <v>1080</v>
+      </c>
+    </row>
+    <row r="393" customFormat="false" ht="89.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A393" s="6" t="s">
+        <v>1081</v>
+      </c>
+      <c r="B393" s="6" t="s">
+        <v>1082</v>
+      </c>
+      <c r="C393" s="6" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="394" customFormat="false" ht="109.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A394" s="6" t="s">
+        <v>1084</v>
+      </c>
+      <c r="B394" s="6" t="s">
+        <v>1085</v>
+      </c>
+      <c r="C394" s="6" t="s">
+        <v>1086</v>
+      </c>
+    </row>
+    <row r="395" customFormat="false" ht="128.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A395" s="6" t="s">
+        <v>1087</v>
+      </c>
+      <c r="B395" s="6" t="s">
+        <v>1088</v>
+      </c>
+      <c r="C395" s="6" t="s">
+        <v>1089</v>
+      </c>
+    </row>
+    <row r="396" customFormat="false" ht="48.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A396" s="6" t="s">
+        <v>1090</v>
+      </c>
+      <c r="B396" s="6" t="s">
+        <v>1091</v>
+      </c>
+      <c r="C396" s="6" t="s">
+        <v>1092</v>
+      </c>
+    </row>
+    <row r="397" customFormat="false" ht="81.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A397" s="6" t="s">
+        <v>1093</v>
+      </c>
+      <c r="B397" s="6" t="s">
+        <v>1094</v>
+      </c>
+      <c r="C397" s="6" t="s">
+        <v>1095</v>
+      </c>
+    </row>
+    <row r="398" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A398" s="6"/>
+      <c r="B398" s="6"/>
+      <c r="C398" s="6"/>
+    </row>
+    <row r="399" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A399" s="6"/>
+      <c r="B399" s="6"/>
+      <c r="C399" s="6"/>
+    </row>
+    <row r="400" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A400" s="6"/>
+      <c r="B400" s="6"/>
+      <c r="C400" s="6"/>
+    </row>
+    <row r="401" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A401" s="6"/>
+      <c r="B401" s="6"/>
+      <c r="C401" s="6"/>
+    </row>
+    <row r="402" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A402" s="6"/>
+      <c r="B402" s="6"/>
+      <c r="C402" s="6"/>
+    </row>
+    <row r="403" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A403" s="6"/>
+      <c r="B403" s="6"/>
+      <c r="C403" s="6"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:C1"/>
@@ -8877,225 +10051,225 @@
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="9" t="s">
-        <v>963</v>
-      </c>
-      <c r="B2" s="9" t="s">
+      <c r="A2" s="8" t="s">
+        <v>1096</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="10"/>
+      <c r="C2" s="9"/>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="10" t="n">
+      <c r="A3" s="9" t="n">
         <v>400</v>
       </c>
-      <c r="B3" s="10" t="s">
-        <v>964</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>965</v>
+      <c r="B3" s="9" t="s">
+        <v>1097</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>1098</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="10" t="n">
+      <c r="A4" s="9" t="n">
         <v>404</v>
       </c>
-      <c r="B4" s="10" t="s">
-        <v>966</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>967</v>
+      <c r="B4" s="9" t="s">
+        <v>1099</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>1100</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="10"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
+      <c r="A5" s="9"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="10"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
+      <c r="A6" s="9"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="10"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
+      <c r="A7" s="9"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="10"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
+      <c r="A8" s="9"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="10"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
+      <c r="A9" s="9"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="10"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
+      <c r="A10" s="9"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="10"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
+      <c r="A11" s="9"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="10"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
+      <c r="A12" s="9"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="10"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
+      <c r="A13" s="9"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="10"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
+      <c r="A14" s="9"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="10"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
+      <c r="A15" s="9"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="10"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="10"/>
+      <c r="A16" s="9"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="10"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
+      <c r="A17" s="9"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="10"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="10"/>
+      <c r="A18" s="9"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="10"/>
-      <c r="B19" s="10"/>
-      <c r="C19" s="10"/>
+      <c r="A19" s="9"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="10"/>
-      <c r="B20" s="10"/>
-      <c r="C20" s="10"/>
+      <c r="A20" s="9"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="10"/>
-      <c r="B21" s="10"/>
-      <c r="C21" s="10"/>
+      <c r="A21" s="9"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="10"/>
-      <c r="B22" s="10"/>
-      <c r="C22" s="10"/>
+      <c r="A22" s="9"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="10"/>
-      <c r="B23" s="10"/>
-      <c r="C23" s="10"/>
+      <c r="A23" s="9"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="9"/>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="10"/>
-      <c r="B24" s="10"/>
-      <c r="C24" s="10"/>
+      <c r="A24" s="9"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="10"/>
-      <c r="B25" s="10"/>
-      <c r="C25" s="10"/>
+      <c r="A25" s="9"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="9"/>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="10"/>
-      <c r="B26" s="10"/>
-      <c r="C26" s="10"/>
+      <c r="A26" s="9"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="10"/>
-      <c r="B27" s="10"/>
-      <c r="C27" s="10"/>
+      <c r="A27" s="9"/>
+      <c r="B27" s="9"/>
+      <c r="C27" s="9"/>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="10"/>
-      <c r="B28" s="10"/>
-      <c r="C28" s="10"/>
+      <c r="A28" s="9"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="9"/>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="10"/>
-      <c r="B29" s="10"/>
-      <c r="C29" s="10"/>
+      <c r="A29" s="9"/>
+      <c r="B29" s="9"/>
+      <c r="C29" s="9"/>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="10"/>
-      <c r="B30" s="10"/>
-      <c r="C30" s="10"/>
+      <c r="A30" s="9"/>
+      <c r="B30" s="9"/>
+      <c r="C30" s="9"/>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="10"/>
-      <c r="B31" s="10"/>
-      <c r="C31" s="10"/>
+      <c r="A31" s="9"/>
+      <c r="B31" s="9"/>
+      <c r="C31" s="9"/>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="10"/>
-      <c r="B32" s="10"/>
-      <c r="C32" s="10"/>
+      <c r="A32" s="9"/>
+      <c r="B32" s="9"/>
+      <c r="C32" s="9"/>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="10"/>
-      <c r="B33" s="10"/>
-      <c r="C33" s="10"/>
+      <c r="A33" s="9"/>
+      <c r="B33" s="9"/>
+      <c r="C33" s="9"/>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="10"/>
-      <c r="B34" s="10"/>
-      <c r="C34" s="10"/>
+      <c r="A34" s="9"/>
+      <c r="B34" s="9"/>
+      <c r="C34" s="9"/>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="10"/>
-      <c r="B35" s="10"/>
-      <c r="C35" s="10"/>
+      <c r="A35" s="9"/>
+      <c r="B35" s="9"/>
+      <c r="C35" s="9"/>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="10"/>
-      <c r="B36" s="10"/>
-      <c r="C36" s="10"/>
+      <c r="A36" s="9"/>
+      <c r="B36" s="9"/>
+      <c r="C36" s="9"/>
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="10"/>
-      <c r="B37" s="10"/>
-      <c r="C37" s="10"/>
+      <c r="A37" s="9"/>
+      <c r="B37" s="9"/>
+      <c r="C37" s="9"/>
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="10"/>
-      <c r="B38" s="10"/>
-      <c r="C38" s="10"/>
+      <c r="A38" s="9"/>
+      <c r="B38" s="9"/>
+      <c r="C38" s="9"/>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="10"/>
-      <c r="B39" s="10"/>
-      <c r="C39" s="10"/>
+      <c r="A39" s="9"/>
+      <c r="B39" s="9"/>
+      <c r="C39" s="9"/>
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="10"/>
-      <c r="B40" s="10"/>
-      <c r="C40" s="10"/>
+      <c r="A40" s="9"/>
+      <c r="B40" s="9"/>
+      <c r="C40" s="9"/>
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="10"/>
-      <c r="B41" s="10"/>
-      <c r="C41" s="10"/>
+      <c r="A41" s="9"/>
+      <c r="B41" s="9"/>
+      <c r="C41" s="9"/>
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="10"/>
-      <c r="B42" s="10"/>
-      <c r="C42" s="10"/>
+      <c r="A42" s="9"/>
+      <c r="B42" s="9"/>
+      <c r="C42" s="9"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
feat: opaque token - script create oauth2_authorization table - create revoke token collection - att documentation
</commit_message>
<xml_diff>
--- a/src/main/resources/docs/especialista-spring-rest.xlsx
+++ b/src/main/resources/docs/especialista-spring-rest.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1222" uniqueCount="1124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1229" uniqueCount="1131">
   <si>
     <t xml:space="preserve">Especialista Spring Rest</t>
   </si>
@@ -5364,8 +5364,37 @@
 - Para fazer requisições basta adicionar o Bearer Token em uma requisição no postman</t>
   </si>
   <si>
-    <t xml:space="preserve">Armazenando Autorizações no
-Banco de Dados</t>
+    <t xml:space="preserve">Bean de Armazenamento de
+Autorizações no Banco de Dados</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Podemos armazenar os tokens no banco de dados para não perdermos o estado da aplicação ao reiniciar
+- Precisamos criar uma tabela para armazenamento das informações do token (a tabela “oauth2_authorization”)
+- No AuthrizationServerConfig adicione o Bean de configuração do JDBC
+@Bean
+ public OAuth2AuthorizationService oauth2AuthorizationService(
+JdbcOperations jdbcOperations, RegisteredClientRepository registeredClientRepository) {…}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27.7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Revogando um Access Token</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Para revogar o token podemos fazer um POST em /oauth2/revoke
+- Devemos passar o form com o token no body (token: {{ACCESS_TOKEN}})
+- Esse endpoint invalidará o token setando “true” na flag metadata.token.invalidated da coluna access_token_metadata</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27.8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Configuração de Token
+JWT no Authorization Server</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27.9</t>
   </si>
   <si>
     <t xml:space="preserve">ERRO</t>
@@ -5500,7 +5529,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -5531,10 +5560,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -5731,8 +5756,8 @@
   </sheetPr>
   <dimension ref="A1:F420"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A403" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A408" activeCellId="0" sqref="A408"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A406" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A410" activeCellId="0" sqref="A410"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10178,7 +10203,7 @@
       <c r="B404" s="6" t="s">
         <v>1111</v>
       </c>
-      <c r="C404" s="8" t="s">
+      <c r="C404" s="6" t="s">
         <v>1112</v>
       </c>
     </row>
@@ -10189,7 +10214,7 @@
       <c r="B405" s="6" t="s">
         <v>1114</v>
       </c>
-      <c r="C405" s="8" t="s">
+      <c r="C405" s="6" t="s">
         <v>1115</v>
       </c>
     </row>
@@ -10200,81 +10225,95 @@
       <c r="B406" s="6" t="s">
         <v>1117</v>
       </c>
-      <c r="C406" s="8" t="s">
+      <c r="C406" s="6" t="s">
         <v>1115</v>
       </c>
     </row>
-    <row r="407" customFormat="false" ht="48.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="407" customFormat="false" ht="88.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A407" s="6" t="s">
         <v>1118</v>
       </c>
-      <c r="B407" s="6"/>
-      <c r="C407" s="8"/>
-    </row>
-    <row r="408" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A408" s="6"/>
-      <c r="B408" s="6"/>
-      <c r="C408" s="8"/>
-    </row>
-    <row r="409" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A409" s="6"/>
+      <c r="B407" s="6" t="s">
+        <v>1119</v>
+      </c>
+      <c r="C407" s="6" t="s">
+        <v>1120</v>
+      </c>
+    </row>
+    <row r="408" customFormat="false" ht="49.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A408" s="6" t="s">
+        <v>1121</v>
+      </c>
+      <c r="B408" s="6" t="s">
+        <v>1122</v>
+      </c>
+      <c r="C408" s="6" t="s">
+        <v>1123</v>
+      </c>
+    </row>
+    <row r="409" customFormat="false" ht="53.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A409" s="6" t="s">
+        <v>1124</v>
+      </c>
       <c r="B409" s="6"/>
-      <c r="C409" s="8"/>
+      <c r="C409" s="6" t="s">
+        <v>1125</v>
+      </c>
     </row>
     <row r="410" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A410" s="6"/>
       <c r="B410" s="6"/>
-      <c r="C410" s="8"/>
+      <c r="C410" s="6"/>
     </row>
     <row r="411" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A411" s="6"/>
       <c r="B411" s="6"/>
-      <c r="C411" s="8"/>
+      <c r="C411" s="6"/>
     </row>
     <row r="412" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A412" s="6"/>
       <c r="B412" s="6"/>
-      <c r="C412" s="8"/>
+      <c r="C412" s="6"/>
     </row>
     <row r="413" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A413" s="6"/>
       <c r="B413" s="6"/>
-      <c r="C413" s="8"/>
+      <c r="C413" s="6"/>
     </row>
     <row r="414" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A414" s="6"/>
       <c r="B414" s="6"/>
-      <c r="C414" s="8"/>
+      <c r="C414" s="6"/>
     </row>
     <row r="415" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A415" s="6"/>
       <c r="B415" s="6"/>
-      <c r="C415" s="8"/>
+      <c r="C415" s="6"/>
     </row>
     <row r="416" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A416" s="6"/>
       <c r="B416" s="6"/>
-      <c r="C416" s="8"/>
+      <c r="C416" s="6"/>
     </row>
     <row r="417" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A417" s="6"/>
       <c r="B417" s="6"/>
-      <c r="C417" s="8"/>
+      <c r="C417" s="6"/>
     </row>
     <row r="418" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A418" s="6"/>
       <c r="B418" s="6"/>
-      <c r="C418" s="8"/>
+      <c r="C418" s="6"/>
     </row>
     <row r="419" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A419" s="6"/>
       <c r="B419" s="6"/>
-      <c r="C419" s="8"/>
+      <c r="C419" s="6"/>
     </row>
     <row r="420" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A420" s="6"/>
       <c r="B420" s="6"/>
-      <c r="C420" s="8"/>
+      <c r="C420" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -10311,225 +10350,225 @@
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="9" t="s">
-        <v>1119</v>
-      </c>
-      <c r="B2" s="9" t="s">
+      <c r="A2" s="8" t="s">
+        <v>1126</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="10"/>
+      <c r="C2" s="9"/>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="10" t="n">
+      <c r="A3" s="9" t="n">
         <v>400</v>
       </c>
-      <c r="B3" s="10" t="s">
-        <v>1120</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>1121</v>
+      <c r="B3" s="9" t="s">
+        <v>1127</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>1128</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="10" t="n">
+      <c r="A4" s="9" t="n">
         <v>404</v>
       </c>
-      <c r="B4" s="10" t="s">
-        <v>1122</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>1123</v>
+      <c r="B4" s="9" t="s">
+        <v>1129</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>1130</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="10"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
+      <c r="A5" s="9"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="10"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
+      <c r="A6" s="9"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="10"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
+      <c r="A7" s="9"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="10"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
+      <c r="A8" s="9"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="10"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
+      <c r="A9" s="9"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="10"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
+      <c r="A10" s="9"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="10"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
+      <c r="A11" s="9"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="10"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
+      <c r="A12" s="9"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="10"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
+      <c r="A13" s="9"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="10"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
+      <c r="A14" s="9"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="10"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
+      <c r="A15" s="9"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="10"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="10"/>
+      <c r="A16" s="9"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="10"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
+      <c r="A17" s="9"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="10"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="10"/>
+      <c r="A18" s="9"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="10"/>
-      <c r="B19" s="10"/>
-      <c r="C19" s="10"/>
+      <c r="A19" s="9"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="10"/>
-      <c r="B20" s="10"/>
-      <c r="C20" s="10"/>
+      <c r="A20" s="9"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="10"/>
-      <c r="B21" s="10"/>
-      <c r="C21" s="10"/>
+      <c r="A21" s="9"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="10"/>
-      <c r="B22" s="10"/>
-      <c r="C22" s="10"/>
+      <c r="A22" s="9"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="10"/>
-      <c r="B23" s="10"/>
-      <c r="C23" s="10"/>
+      <c r="A23" s="9"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="9"/>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="10"/>
-      <c r="B24" s="10"/>
-      <c r="C24" s="10"/>
+      <c r="A24" s="9"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="10"/>
-      <c r="B25" s="10"/>
-      <c r="C25" s="10"/>
+      <c r="A25" s="9"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="9"/>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="10"/>
-      <c r="B26" s="10"/>
-      <c r="C26" s="10"/>
+      <c r="A26" s="9"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="10"/>
-      <c r="B27" s="10"/>
-      <c r="C27" s="10"/>
+      <c r="A27" s="9"/>
+      <c r="B27" s="9"/>
+      <c r="C27" s="9"/>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="10"/>
-      <c r="B28" s="10"/>
-      <c r="C28" s="10"/>
+      <c r="A28" s="9"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="9"/>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="10"/>
-      <c r="B29" s="10"/>
-      <c r="C29" s="10"/>
+      <c r="A29" s="9"/>
+      <c r="B29" s="9"/>
+      <c r="C29" s="9"/>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="10"/>
-      <c r="B30" s="10"/>
-      <c r="C30" s="10"/>
+      <c r="A30" s="9"/>
+      <c r="B30" s="9"/>
+      <c r="C30" s="9"/>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="10"/>
-      <c r="B31" s="10"/>
-      <c r="C31" s="10"/>
+      <c r="A31" s="9"/>
+      <c r="B31" s="9"/>
+      <c r="C31" s="9"/>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="10"/>
-      <c r="B32" s="10"/>
-      <c r="C32" s="10"/>
+      <c r="A32" s="9"/>
+      <c r="B32" s="9"/>
+      <c r="C32" s="9"/>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="10"/>
-      <c r="B33" s="10"/>
-      <c r="C33" s="10"/>
+      <c r="A33" s="9"/>
+      <c r="B33" s="9"/>
+      <c r="C33" s="9"/>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="10"/>
-      <c r="B34" s="10"/>
-      <c r="C34" s="10"/>
+      <c r="A34" s="9"/>
+      <c r="B34" s="9"/>
+      <c r="C34" s="9"/>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="10"/>
-      <c r="B35" s="10"/>
-      <c r="C35" s="10"/>
+      <c r="A35" s="9"/>
+      <c r="B35" s="9"/>
+      <c r="C35" s="9"/>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="10"/>
-      <c r="B36" s="10"/>
-      <c r="C36" s="10"/>
+      <c r="A36" s="9"/>
+      <c r="B36" s="9"/>
+      <c r="C36" s="9"/>
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="10"/>
-      <c r="B37" s="10"/>
-      <c r="C37" s="10"/>
+      <c r="A37" s="9"/>
+      <c r="B37" s="9"/>
+      <c r="C37" s="9"/>
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="10"/>
-      <c r="B38" s="10"/>
-      <c r="C38" s="10"/>
+      <c r="A38" s="9"/>
+      <c r="B38" s="9"/>
+      <c r="C38" s="9"/>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="10"/>
-      <c r="B39" s="10"/>
-      <c r="C39" s="10"/>
+      <c r="A39" s="9"/>
+      <c r="B39" s="9"/>
+      <c r="C39" s="9"/>
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="10"/>
-      <c r="B40" s="10"/>
-      <c r="C40" s="10"/>
+      <c r="A40" s="9"/>
+      <c r="B40" s="9"/>
+      <c r="C40" s="9"/>
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="10"/>
-      <c r="B41" s="10"/>
-      <c r="C41" s="10"/>
+      <c r="A41" s="9"/>
+      <c r="B41" s="9"/>
+      <c r="C41" s="9"/>
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="10"/>
-      <c r="B42" s="10"/>
-      <c r="C42" s="10"/>
+      <c r="A42" s="9"/>
+      <c r="B42" s="9"/>
+      <c r="C42" s="9"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
feat: jwt token - authorization server config - create oauth jwks token collection - att documentation
</commit_message>
<xml_diff>
--- a/src/main/resources/docs/especialista-spring-rest.xlsx
+++ b/src/main/resources/docs/especialista-spring-rest.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1229" uniqueCount="1131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1237" uniqueCount="1138">
   <si>
     <t xml:space="preserve">Especialista Spring Rest</t>
   </si>
@@ -5394,7 +5394,40 @@
 JWT no Authorization Server</t>
   </si>
   <si>
+    <t xml:space="preserve">'- O token JWT é transparente ou seja guarda informações da requisição em seu payload
+- Em RegisteredClient devemos alterar o tipo do token para OAuth2TokenFormat.SELF_CONTAINED que será nosso token transparente
+- Após essa configuração é necessário adicionar alguns beans</t>
+  </si>
+  <si>
     <t xml:space="preserve">27.9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bean de Assinatura do JWT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'- Bean do tipo JWK Set com par de chaves públicas e privadas
+- Adicione o Bean no AuthorizationServerConfig
+@Bean
+    public JWKSource&lt;SecurityContext&gt; jwkSource(JwtKeyStoreProperties jwtKeyStoreProperties) {…}
+- Esse Bean será responsável por configurar todas as funcionalidades que dependem da chave publica e privada para criação do token
+- Leitura do JKS como Resource base64 do application properties, disponibilização da chava para uso
+- Podemos consultar a chave pública no endpoint /oauth2/jwks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Configurando o ResourceServer
+Com Token JWT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'- Precisamos configurar para que o Resource Server ao receber o token Jwt verifique a sua assinatura via chave pública via endpoint jwks
+- No metodo resourceServerFilterChain altere o http...oauth2ResourceServer().jwt();
+- No application properties defina qual será a url do authorization-server para chave publica
+spring.security.oauth2.resourceserver.jwt.jwk-set-uri=http://localhost:9000/oauth2/jwks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27.10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.</t>
   </si>
   <si>
     <t xml:space="preserve">ERRO</t>
@@ -5756,8 +5789,8 @@
   </sheetPr>
   <dimension ref="A1:F420"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A406" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A410" activeCellId="0" sqref="A410"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A409" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B414" activeCellId="0" sqref="B414"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10255,23 +10288,39 @@
       <c r="A409" s="6" t="s">
         <v>1124</v>
       </c>
-      <c r="B409" s="6"/>
+      <c r="B409" s="6" t="s">
+        <v>1125</v>
+      </c>
       <c r="C409" s="6" t="s">
-        <v>1125</v>
-      </c>
-    </row>
-    <row r="410" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A410" s="6"/>
-      <c r="B410" s="6"/>
-      <c r="C410" s="6"/>
-    </row>
-    <row r="411" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A411" s="6"/>
-      <c r="B411" s="6"/>
-      <c r="C411" s="6"/>
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="410" customFormat="false" ht="110.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A410" s="6" t="s">
+        <v>1127</v>
+      </c>
+      <c r="B410" s="6" t="s">
+        <v>1128</v>
+      </c>
+      <c r="C410" s="6" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="411" customFormat="false" ht="66.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A411" s="6" t="s">
+        <v>1129</v>
+      </c>
+      <c r="B411" s="6" t="s">
+        <v>1130</v>
+      </c>
+      <c r="C411" s="6" t="s">
+        <v>1131</v>
+      </c>
     </row>
     <row r="412" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A412" s="6"/>
+      <c r="A412" s="6" t="s">
+        <v>1132</v>
+      </c>
       <c r="B412" s="6"/>
       <c r="C412" s="6"/>
     </row>
@@ -10351,7 +10400,7 @@
   <sheetData>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="8" t="s">
-        <v>1126</v>
+        <v>1133</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>2</v>
@@ -10363,10 +10412,10 @@
         <v>400</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>1127</v>
+        <v>1134</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>1128</v>
+        <v>1135</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10374,10 +10423,10 @@
         <v>404</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>1129</v>
+        <v>1136</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>1130</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
feat: authorization code flow - authorization server config - resource server connfig - create authorization code collection - adjust jpa user serialization - att documentation
</commit_message>
<xml_diff>
--- a/src/main/resources/docs/especialista-spring-rest.xlsx
+++ b/src/main/resources/docs/especialista-spring-rest.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1237" uniqueCount="1138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1244" uniqueCount="1145">
   <si>
     <t xml:space="preserve">Especialista Spring Rest</t>
   </si>
@@ -5427,7 +5427,42 @@
     <t xml:space="preserve">27.10</t>
   </si>
   <si>
-    <t xml:space="preserve">.</t>
+    <t xml:space="preserve">Fluxo Authorization Code
+Com PKCE e SHA256</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Primeiro devemos habilitar a tela de login em filterChain no AuthorizationServerConfig e ResourceServerConfig
+http.formLogin(Customizer.withDefaults()).build();
+- Faça a declaração dos outros RegisteredClients no AuthServerConfig com AuthMethod CLIENT_SECRET_BASIC, grantType AUTHORIZATION_CODE
+E com redirectUri para localhost:9000/authorized
+- Por fim adicionar na lista de clients InMemoryRegisteredClientRepository(Arrays.asList(algafoodbackend, algafoodweb));</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27.11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Testando o Fluxo
+Auth Code + PKCE + SHA256</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Vamos construir a url no postman no path /oauth2/authorize e passando os parâmetros:
+* response_type = code (Para fluxo Auth Code)
+* client_id = algafood-web
+* state = AbCXyZ (Estado gerado pelo front)
+* redirect_uri= 127.0.0.1:9000/authorized
+* scope=READ WRITE
+* code_challenge=BqZff7HQezJuHzCsBKl1Gq5bG3NoLcG3istqwIc-kJ0 (Pode ser simulado no site Online /pkce-generator/)
+* code_challenge_method=S256
+- Com isso teremos o authorization code e conseguimos solicitar o token no path /oauth2/token</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27.12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implementando o Refresh Token</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27.13</t>
   </si>
   <si>
     <t xml:space="preserve">ERRO</t>
@@ -5789,8 +5824,8 @@
   </sheetPr>
   <dimension ref="A1:F420"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A409" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B414" activeCellId="0" sqref="B414"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A410" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A415" activeCellId="0" sqref="A415"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10317,22 +10352,36 @@
         <v>1131</v>
       </c>
     </row>
-    <row r="412" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="412" customFormat="false" ht="92.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A412" s="6" t="s">
         <v>1132</v>
       </c>
-      <c r="B412" s="6"/>
-      <c r="C412" s="6"/>
-    </row>
-    <row r="413" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A413" s="6"/>
-      <c r="B413" s="6"/>
-      <c r="C413" s="6"/>
+      <c r="B412" s="6" t="s">
+        <v>1133</v>
+      </c>
+      <c r="C412" s="6" t="s">
+        <v>1134</v>
+      </c>
+    </row>
+    <row r="413" customFormat="false" ht="119.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A413" s="6" t="s">
+        <v>1135</v>
+      </c>
+      <c r="B413" s="6" t="s">
+        <v>1136</v>
+      </c>
+      <c r="C413" s="6" t="s">
+        <v>1137</v>
+      </c>
     </row>
     <row r="414" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A414" s="6"/>
+      <c r="A414" s="6" t="s">
+        <v>1138</v>
+      </c>
       <c r="B414" s="6"/>
-      <c r="C414" s="6"/>
+      <c r="C414" s="6" t="s">
+        <v>1139</v>
+      </c>
     </row>
     <row r="415" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A415" s="6"/>
@@ -10400,7 +10449,7 @@
   <sheetData>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="8" t="s">
-        <v>1133</v>
+        <v>1140</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>2</v>
@@ -10412,10 +10461,10 @@
         <v>400</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>1134</v>
+        <v>1141</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>1135</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10423,10 +10472,10 @@
         <v>404</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>1136</v>
+        <v>1143</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>1137</v>
+        <v>1144</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
feat: refresh token - authorization server config - create refresh token collection
</commit_message>
<xml_diff>
--- a/src/main/resources/docs/especialista-spring-rest.xlsx
+++ b/src/main/resources/docs/especialista-spring-rest.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1244" uniqueCount="1145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1248" uniqueCount="1148">
   <si>
     <t xml:space="preserve">Especialista Spring Rest</t>
   </si>
@@ -5462,7 +5462,25 @@
     <t xml:space="preserve">Implementando o Refresh Token</t>
   </si>
   <si>
+    <t xml:space="preserve">- Para a utilização do Refresh Token devemos adicionar o parâmetro no RegisteredClient
+.authorizationGrantType(AuthorizationGrantType.REFRESH_TOKEN)
+- Podemos configura o tempo de expiração e seu reuso
+.refreshTokenTimeToLive(Duration.ofDays(1))
+.reuseRefreshTokens(false)</t>
+  </si>
+  <si>
     <t xml:space="preserve">27.13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Script para preencher 
+Refresh Token</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Para o refresh token podemos utilizar o seguinte script:
+var jsonData = pm.response.json();
+pm.environment.set("ACCESS_TOKEN", jsonData.access_token);
+pm.environment.set("REFRESH_TOKEN", jsonData.refresh_token);
+- Utilizamos o path /oauth2/token com o grant_type refresh_token seguido do próprio refresh_token como form mno body</t>
   </si>
   <si>
     <t xml:space="preserve">ERRO</t>
@@ -5824,8 +5842,8 @@
   </sheetPr>
   <dimension ref="A1:F420"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A410" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A415" activeCellId="0" sqref="A415"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A413" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B416" activeCellId="0" sqref="B416"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10374,19 +10392,27 @@
         <v>1137</v>
       </c>
     </row>
-    <row r="414" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="414" customFormat="false" ht="76.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A414" s="6" t="s">
         <v>1138</v>
       </c>
-      <c r="B414" s="6"/>
+      <c r="B414" s="6" t="s">
+        <v>1139</v>
+      </c>
       <c r="C414" s="6" t="s">
-        <v>1139</v>
-      </c>
-    </row>
-    <row r="415" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A415" s="6"/>
-      <c r="B415" s="6"/>
-      <c r="C415" s="6"/>
+        <v>1140</v>
+      </c>
+    </row>
+    <row r="415" customFormat="false" ht="75.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A415" s="6" t="s">
+        <v>1141</v>
+      </c>
+      <c r="B415" s="6" t="s">
+        <v>1142</v>
+      </c>
+      <c r="C415" s="6" t="s">
+        <v>1140</v>
+      </c>
     </row>
     <row r="416" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A416" s="6"/>
@@ -10449,7 +10475,7 @@
   <sheetData>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="8" t="s">
-        <v>1140</v>
+        <v>1143</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>2</v>
@@ -10461,10 +10487,10 @@
         <v>400</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>1141</v>
+        <v>1144</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>1142</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10472,10 +10498,10 @@
         <v>404</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>1143</v>
+        <v>1146</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>1144</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
feat: claims customizer - authorization server config - cors config - att documentation
</commit_message>
<xml_diff>
--- a/src/main/resources/docs/especialista-spring-rest.xlsx
+++ b/src/main/resources/docs/especialista-spring-rest.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1248" uniqueCount="1148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1251" uniqueCount="1151">
   <si>
     <t xml:space="preserve">Especialista Spring Rest</t>
   </si>
@@ -5481,6 +5481,18 @@
 pm.environment.set("ACCESS_TOKEN", jsonData.access_token);
 pm.environment.set("REFRESH_TOKEN", jsonData.refresh_token);
 - Utilizamos o path /oauth2/token com o grant_type refresh_token seguido do próprio refresh_token como form mno body</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Customização do Auth User</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'- Para customizar as permissões do usuário usando Claims precisamos criar um @Bean de TokenCustomizer
+- No AuthorizationServerConfig crie o bean de customização
+@Bean
+    public OAuth2TokenCustomizer&lt;JwtEncodingContext&gt; jwtCustomizer(UsuarioRepository usuarioRepository) {…}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27.14</t>
   </si>
   <si>
     <t xml:space="preserve">ERRO</t>
@@ -10414,10 +10426,16 @@
         <v>1140</v>
       </c>
     </row>
-    <row r="416" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A416" s="6"/>
-      <c r="B416" s="6"/>
-      <c r="C416" s="6"/>
+    <row r="416" customFormat="false" ht="54.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A416" s="6" t="s">
+        <v>1143</v>
+      </c>
+      <c r="B416" s="6" t="s">
+        <v>1144</v>
+      </c>
+      <c r="C416" s="6" t="s">
+        <v>1145</v>
+      </c>
     </row>
     <row r="417" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A417" s="6"/>
@@ -10475,7 +10493,7 @@
   <sheetData>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="8" t="s">
-        <v>1143</v>
+        <v>1146</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>2</v>
@@ -10487,10 +10505,10 @@
         <v>400</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>1144</v>
+        <v>1147</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10498,10 +10516,10 @@
         <v>404</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>1147</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
feat: jwt customizer - authorization server config - att version path collections - att documentation
</commit_message>
<xml_diff>
--- a/src/main/resources/docs/especialista-spring-rest.xlsx
+++ b/src/main/resources/docs/especialista-spring-rest.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1251" uniqueCount="1151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1254" uniqueCount="1154">
   <si>
     <t xml:space="preserve">Especialista Spring Rest</t>
   </si>
@@ -5493,6 +5493,19 @@
   </si>
   <si>
     <t xml:space="preserve">27.14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lendo as Claims Customizadas no 
+Resource Server Config</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'- Para fazer a leitura do jwt customizados precisamos criar um JwtAuthenticationConverter no ResourceServerConfig
+private JwtAuthenticationConverter jwtAuthenticationConverter() {…}
+- No SecurityFilterChain podemos definir nosso converter:
+.oauth2ResourceServer().jwt().jwtAuthenticationConverter(jwtAuthenticationConverter());</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27.15</t>
   </si>
   <si>
     <t xml:space="preserve">ERRO</t>
@@ -5855,7 +5868,7 @@
   <dimension ref="A1:F420"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A413" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B416" activeCellId="0" sqref="B416"/>
+      <selection pane="topLeft" activeCell="B418" activeCellId="0" sqref="B418"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10437,10 +10450,16 @@
         <v>1145</v>
       </c>
     </row>
-    <row r="417" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A417" s="6"/>
-      <c r="B417" s="6"/>
-      <c r="C417" s="6"/>
+    <row r="417" customFormat="false" ht="65.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A417" s="6" t="s">
+        <v>1146</v>
+      </c>
+      <c r="B417" s="6" t="s">
+        <v>1147</v>
+      </c>
+      <c r="C417" s="6" t="s">
+        <v>1148</v>
+      </c>
     </row>
     <row r="418" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A418" s="6"/>
@@ -10493,7 +10512,7 @@
   <sheetData>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="8" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>2</v>
@@ -10505,10 +10524,10 @@
         <v>400</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>1147</v>
+        <v>1150</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>1148</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10516,10 +10535,10 @@
         <v>404</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>1149</v>
+        <v>1152</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>1150</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
feat: registered clients jdbc - create table oauth2 clients - remove old table oauth client details - adding cliets by after migrate sql - authorization server config with jdbc repository - att collections - att documentation
</commit_message>
<xml_diff>
--- a/src/main/resources/docs/especialista-spring-rest.xlsx
+++ b/src/main/resources/docs/especialista-spring-rest.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1254" uniqueCount="1154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1257" uniqueCount="1157">
   <si>
     <t xml:space="preserve">Especialista Spring Rest</t>
   </si>
@@ -5506,6 +5506,32 @@
   </si>
   <si>
     <t xml:space="preserve">27.15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Armazenamento em Banco
+Clients OAuth2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'- Para que isso seja possivel é necessário a criação da tabela oauth2_registered_client
+- Em authorizationServerConfig em vez de utilizar InMemory devemos utilizar um JdbcRegisteredClientRepository
+- E cadastrar os clientes conforme os campos
+OBS.: Podemos subir nossa aplicação a primeira vez e cadastrar os clientes que já temos (Não se esqueça de remover depois):
+RegisteredClient foodanalytics = RegisteredClient.withId("3")
+.clientId("foodanalytics")
+.clientSecret(passwordEncoder.encode("web123"))
+.clientAuthenticationMethod(ClientAuthenticationMethod.CLIENT_SECRET_BASIC)
+.authorizationGrantType(AuthorizationGrantType.AUTHORIZATION_CODE)
+ .scope("READ").scope("WRITE").tokenSettings(TokenSettings.builder()
+                        .accessTokenFormat(OAuth2TokenFormat.SELF_CONTAINED)
+.accessTokenTimeToLive(Duration.ofMinutes(30)).build())
+.redirectUri("http://127.0.0.1:8082")
+.clientSettings(ClientSettings.builder()
+.requireAuthorizationConsent(false).build()).build();
+        JdbcRegisteredClientRepository repository = new JdbcRegisteredClientRepository(jdbcOperations);
+        Repository.save(foodanalytics);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27.16</t>
   </si>
   <si>
     <t xml:space="preserve">ERRO</t>
@@ -5867,8 +5893,8 @@
   </sheetPr>
   <dimension ref="A1:F420"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A413" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B418" activeCellId="0" sqref="B418"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A417" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B425" activeCellId="0" sqref="B425"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10461,10 +10487,16 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="418" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A418" s="6"/>
-      <c r="B418" s="6"/>
-      <c r="C418" s="6"/>
+    <row r="418" customFormat="false" ht="237.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A418" s="6" t="s">
+        <v>1149</v>
+      </c>
+      <c r="B418" s="6" t="s">
+        <v>1150</v>
+      </c>
+      <c r="C418" s="6" t="s">
+        <v>1151</v>
+      </c>
     </row>
     <row r="419" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A419" s="6"/>
@@ -10512,7 +10544,7 @@
   <sheetData>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="8" t="s">
-        <v>1149</v>
+        <v>1152</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>2</v>
@@ -10524,10 +10556,10 @@
         <v>400</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>1150</v>
+        <v>1153</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>1151</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10535,10 +10567,10 @@
         <v>404</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>1152</v>
+        <v>1155</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>1153</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
feat: custom login access page - web mvc config - authorization server config - att documentation
</commit_message>
<xml_diff>
--- a/src/main/resources/docs/especialista-spring-rest.xlsx
+++ b/src/main/resources/docs/especialista-spring-rest.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1257" uniqueCount="1157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1263" uniqueCount="1163">
   <si>
     <t xml:space="preserve">Especialista Spring Rest</t>
   </si>
@@ -5532,6 +5532,32 @@
   </si>
   <si>
     <t xml:space="preserve">27.16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Customizando a tela de Login</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Para customizar a pagina de login basta adicionarmos um comando no filterChain apontando para a tela de login no ResourceServer e no AuthorizationServer
+http.formLogin(customizer -&gt; customizer.loginPage("/oauth/login")).build();
+- Necessário a criação de um WebMvcConfig para fazer a requisição em /login vincular ao local uma pagina
+@Configuration
+public class WebMvcConfig implements WebMvcConfigurer {
+@Override
+public void addViewControllers( ViewControllerRegistry registry) {
+registry.addViewController("/login").setViewName("pages/login");
+registry.setOrder(Ordered.HIGHEST_PRECEDENCE);}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27.17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Customizando a tela de consentimento do OAuth2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- No Authorization Service devemos adicionar um Bean para customização de consent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27.18</t>
   </si>
   <si>
     <t xml:space="preserve">ERRO</t>
@@ -5666,7 +5692,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -5697,6 +5723,14 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -5891,10 +5925,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F420"/>
+  <dimension ref="A1:F425"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A417" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B425" activeCellId="0" sqref="B425"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A418" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B420" activeCellId="0" sqref="B420"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10498,15 +10532,52 @@
         <v>1151</v>
       </c>
     </row>
-    <row r="419" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A419" s="6"/>
-      <c r="B419" s="6"/>
-      <c r="C419" s="6"/>
-    </row>
-    <row r="420" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A420" s="6"/>
-      <c r="B420" s="6"/>
-      <c r="C420" s="6"/>
+    <row r="419" customFormat="false" ht="137.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A419" s="6" t="s">
+        <v>1152</v>
+      </c>
+      <c r="B419" s="6" t="s">
+        <v>1153</v>
+      </c>
+      <c r="C419" s="6" t="s">
+        <v>1154</v>
+      </c>
+    </row>
+    <row r="420" customFormat="false" ht="54.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A420" s="6" t="s">
+        <v>1155</v>
+      </c>
+      <c r="B420" s="6" t="s">
+        <v>1156</v>
+      </c>
+      <c r="C420" s="6" t="s">
+        <v>1157</v>
+      </c>
+    </row>
+    <row r="421" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A421" s="8"/>
+      <c r="B421" s="8"/>
+      <c r="C421" s="9"/>
+    </row>
+    <row r="422" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A422" s="8"/>
+      <c r="B422" s="8"/>
+      <c r="C422" s="9"/>
+    </row>
+    <row r="423" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A423" s="8"/>
+      <c r="B423" s="8"/>
+      <c r="C423" s="9"/>
+    </row>
+    <row r="424" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A424" s="8"/>
+      <c r="B424" s="8"/>
+      <c r="C424" s="9"/>
+    </row>
+    <row r="425" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A425" s="8"/>
+      <c r="B425" s="8"/>
+      <c r="C425" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -10543,225 +10614,225 @@
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="8" t="s">
-        <v>1152</v>
-      </c>
-      <c r="B2" s="8" t="s">
+      <c r="A2" s="10" t="s">
+        <v>1158</v>
+      </c>
+      <c r="B2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="9"/>
+      <c r="C2" s="11"/>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="9" t="n">
+      <c r="A3" s="11" t="n">
         <v>400</v>
       </c>
-      <c r="B3" s="9" t="s">
-        <v>1153</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>1154</v>
+      <c r="B3" s="11" t="s">
+        <v>1159</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>1160</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="9" t="n">
+      <c r="A4" s="11" t="n">
         <v>404</v>
       </c>
-      <c r="B4" s="9" t="s">
-        <v>1155</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>1156</v>
+      <c r="B4" s="11" t="s">
+        <v>1161</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>1162</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="9"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
+      <c r="A5" s="11"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="9"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
+      <c r="A6" s="11"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="9"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
+      <c r="A7" s="11"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="9"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
+      <c r="A8" s="11"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="9"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
+      <c r="A9" s="11"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="9"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
+      <c r="A10" s="11"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="9"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
+      <c r="A11" s="11"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="9"/>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
+      <c r="A12" s="11"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="9"/>
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
+      <c r="A13" s="11"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="9"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
+      <c r="A14" s="11"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="9"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
+      <c r="A15" s="11"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="9"/>
-      <c r="B16" s="9"/>
-      <c r="C16" s="9"/>
+      <c r="A16" s="11"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="9"/>
-      <c r="B17" s="9"/>
-      <c r="C17" s="9"/>
+      <c r="A17" s="11"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="9"/>
-      <c r="B18" s="9"/>
-      <c r="C18" s="9"/>
+      <c r="A18" s="11"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="9"/>
-      <c r="B19" s="9"/>
-      <c r="C19" s="9"/>
+      <c r="A19" s="11"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="9"/>
-      <c r="B20" s="9"/>
-      <c r="C20" s="9"/>
+      <c r="A20" s="11"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="11"/>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="9"/>
-      <c r="B21" s="9"/>
-      <c r="C21" s="9"/>
+      <c r="A21" s="11"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="11"/>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="9"/>
-      <c r="B22" s="9"/>
-      <c r="C22" s="9"/>
+      <c r="A22" s="11"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="11"/>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="9"/>
-      <c r="B23" s="9"/>
-      <c r="C23" s="9"/>
+      <c r="A23" s="11"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="11"/>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="9"/>
-      <c r="B24" s="9"/>
-      <c r="C24" s="9"/>
+      <c r="A24" s="11"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="11"/>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="9"/>
-      <c r="B25" s="9"/>
-      <c r="C25" s="9"/>
+      <c r="A25" s="11"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="9"/>
-      <c r="B26" s="9"/>
-      <c r="C26" s="9"/>
+      <c r="A26" s="11"/>
+      <c r="B26" s="11"/>
+      <c r="C26" s="11"/>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="9"/>
-      <c r="B27" s="9"/>
-      <c r="C27" s="9"/>
+      <c r="A27" s="11"/>
+      <c r="B27" s="11"/>
+      <c r="C27" s="11"/>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="9"/>
-      <c r="B28" s="9"/>
-      <c r="C28" s="9"/>
+      <c r="A28" s="11"/>
+      <c r="B28" s="11"/>
+      <c r="C28" s="11"/>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="9"/>
-      <c r="B29" s="9"/>
-      <c r="C29" s="9"/>
+      <c r="A29" s="11"/>
+      <c r="B29" s="11"/>
+      <c r="C29" s="11"/>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="9"/>
-      <c r="B30" s="9"/>
-      <c r="C30" s="9"/>
+      <c r="A30" s="11"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="11"/>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="9"/>
-      <c r="B31" s="9"/>
-      <c r="C31" s="9"/>
+      <c r="A31" s="11"/>
+      <c r="B31" s="11"/>
+      <c r="C31" s="11"/>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="9"/>
-      <c r="B32" s="9"/>
-      <c r="C32" s="9"/>
+      <c r="A32" s="11"/>
+      <c r="B32" s="11"/>
+      <c r="C32" s="11"/>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="9"/>
-      <c r="B33" s="9"/>
-      <c r="C33" s="9"/>
+      <c r="A33" s="11"/>
+      <c r="B33" s="11"/>
+      <c r="C33" s="11"/>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="9"/>
-      <c r="B34" s="9"/>
-      <c r="C34" s="9"/>
+      <c r="A34" s="11"/>
+      <c r="B34" s="11"/>
+      <c r="C34" s="11"/>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="9"/>
-      <c r="B35" s="9"/>
-      <c r="C35" s="9"/>
+      <c r="A35" s="11"/>
+      <c r="B35" s="11"/>
+      <c r="C35" s="11"/>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="9"/>
-      <c r="B36" s="9"/>
-      <c r="C36" s="9"/>
+      <c r="A36" s="11"/>
+      <c r="B36" s="11"/>
+      <c r="C36" s="11"/>
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="9"/>
-      <c r="B37" s="9"/>
-      <c r="C37" s="9"/>
+      <c r="A37" s="11"/>
+      <c r="B37" s="11"/>
+      <c r="C37" s="11"/>
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="9"/>
-      <c r="B38" s="9"/>
-      <c r="C38" s="9"/>
+      <c r="A38" s="11"/>
+      <c r="B38" s="11"/>
+      <c r="C38" s="11"/>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="9"/>
-      <c r="B39" s="9"/>
-      <c r="C39" s="9"/>
+      <c r="A39" s="11"/>
+      <c r="B39" s="11"/>
+      <c r="C39" s="11"/>
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="9"/>
-      <c r="B40" s="9"/>
-      <c r="C40" s="9"/>
+      <c r="A40" s="11"/>
+      <c r="B40" s="11"/>
+      <c r="C40" s="11"/>
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="9"/>
-      <c r="B41" s="9"/>
-      <c r="C41" s="9"/>
+      <c r="A41" s="11"/>
+      <c r="B41" s="11"/>
+      <c r="C41" s="11"/>
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="9"/>
-      <c r="B42" s="9"/>
-      <c r="C42" s="9"/>
+      <c r="A42" s="11"/>
+      <c r="B42" s="11"/>
+      <c r="C42" s="11"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
feat: custom consent service - create table oauth2_authorization_consent - persist consent in database - create controller to redirect page - resource server with authorization in oauth2 path - att approval html - att documentation
</commit_message>
<xml_diff>
--- a/src/main/resources/docs/especialista-spring-rest.xlsx
+++ b/src/main/resources/docs/especialista-spring-rest.xlsx
@@ -5554,7 +5554,16 @@
     <t xml:space="preserve">Customizando a tela de consentimento do OAuth2</t>
   </si>
   <si>
-    <t xml:space="preserve">- No Authorization Service devemos adicionar um Bean para customização de consent</t>
+    <t xml:space="preserve">'- No Authorization Service devemos adicionar um Bean para customização de consent
+@Bean
+public OAuth2AuthorizationConsentService consentService() {…}
+- No FilterChain precisamos customizar as configurações e não utilizar a applyDefaultSecurity(http)
+- Após isso é necessário a criação de um controller para encaminhar as requisições então criaremo um AuthorizationConsetController
+- Para armazenar as consessões no banco de dados devemos ajustar o ConsentService
+@Bean
+public OAuth2AuthorizationConsentService consentService(
+JdbcOperations jdbcOperations,RegisteredClientRepository clientRepository) {…}
+- E criar a tabela oauth2_authorization_consent  com db migration</t>
   </si>
   <si>
     <t xml:space="preserve">27.18</t>
@@ -5927,8 +5936,8 @@
   </sheetPr>
   <dimension ref="A1:F425"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A418" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B420" activeCellId="0" sqref="B420"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A419" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B427" activeCellId="0" sqref="B427"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10543,7 +10552,7 @@
         <v>1154</v>
       </c>
     </row>
-    <row r="420" customFormat="false" ht="54.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="420" customFormat="false" ht="156.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A420" s="6" t="s">
         <v>1155</v>
       </c>

</xml_diff>

<commit_message>
feat: consent clients page - adjust clients name in after migrate sql - create query to list consent clients - create consent query service - create controller with consent path - create authorized clients html - att documentation
</commit_message>
<xml_diff>
--- a/src/main/resources/docs/especialista-spring-rest.xlsx
+++ b/src/main/resources/docs/especialista-spring-rest.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1263" uniqueCount="1163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1266" uniqueCount="1166">
   <si>
     <t xml:space="preserve">Especialista Spring Rest</t>
   </si>
@@ -5567,6 +5567,23 @@
   </si>
   <si>
     <t xml:space="preserve">27.18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Criando página de clientes consentidos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Essa customização disponível NÃO é compatível com redis ou inmemory, somente com a persistência no JDBC
+- criar query com clients consentidos
+- criar interface para o repository OAuth2AuthorizationQueryService
+- criar serviço JdbcOAuth2AuthorizationQueryService
+- criar controller para disponilizar clients com path /oauth2/authorized-clients
+- criar uma pagina authorized-clients.html
+- criar um bean para iniciar o service:
+@Bean
+public OAuth2AuthorizationQueryService auth2AuthorizationQueryService(JdbcOperations jdbcOperations) {…}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27.20</t>
   </si>
   <si>
     <t xml:space="preserve">ERRO</t>
@@ -5701,7 +5718,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -5734,11 +5751,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5937,7 +5950,7 @@
   <dimension ref="A1:F425"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A419" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B427" activeCellId="0" sqref="B427"/>
+      <selection pane="topLeft" activeCell="B421" activeCellId="0" sqref="B421"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10563,30 +10576,36 @@
         <v>1157</v>
       </c>
     </row>
-    <row r="421" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A421" s="8"/>
-      <c r="B421" s="8"/>
-      <c r="C421" s="9"/>
+    <row r="421" customFormat="false" ht="110.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A421" s="6" t="s">
+        <v>1158</v>
+      </c>
+      <c r="B421" s="6" t="s">
+        <v>1159</v>
+      </c>
+      <c r="C421" s="8" t="s">
+        <v>1160</v>
+      </c>
     </row>
     <row r="422" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A422" s="8"/>
-      <c r="B422" s="8"/>
-      <c r="C422" s="9"/>
+      <c r="A422" s="6"/>
+      <c r="B422" s="6"/>
+      <c r="C422" s="8"/>
     </row>
     <row r="423" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A423" s="8"/>
-      <c r="B423" s="8"/>
-      <c r="C423" s="9"/>
+      <c r="A423" s="6"/>
+      <c r="B423" s="6"/>
+      <c r="C423" s="8"/>
     </row>
     <row r="424" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A424" s="8"/>
-      <c r="B424" s="8"/>
-      <c r="C424" s="9"/>
+      <c r="A424" s="6"/>
+      <c r="B424" s="6"/>
+      <c r="C424" s="8"/>
     </row>
     <row r="425" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A425" s="8"/>
-      <c r="B425" s="8"/>
-      <c r="C425" s="9"/>
+      <c r="A425" s="6"/>
+      <c r="B425" s="6"/>
+      <c r="C425" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -10623,225 +10642,225 @@
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="10" t="s">
-        <v>1158</v>
-      </c>
-      <c r="B2" s="10" t="s">
+      <c r="A2" s="9" t="s">
+        <v>1161</v>
+      </c>
+      <c r="B2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="11"/>
+      <c r="C2" s="10"/>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="11" t="n">
+      <c r="A3" s="10" t="n">
         <v>400</v>
       </c>
-      <c r="B3" s="11" t="s">
-        <v>1159</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>1160</v>
+      <c r="B3" s="10" t="s">
+        <v>1162</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>1163</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="11" t="n">
+      <c r="A4" s="10" t="n">
         <v>404</v>
       </c>
-      <c r="B4" s="11" t="s">
-        <v>1161</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>1162</v>
+      <c r="B4" s="10" t="s">
+        <v>1164</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>1165</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
+      <c r="A5" s="10"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="11"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
+      <c r="A6" s="10"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="11"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
+      <c r="A7" s="10"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="11"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
+      <c r="A8" s="10"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="11"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
+      <c r="A9" s="10"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="11"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
+      <c r="A10" s="10"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="11"/>
-      <c r="B11" s="11"/>
-      <c r="C11" s="11"/>
+      <c r="A11" s="10"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="11"/>
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
+      <c r="A12" s="10"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="11"/>
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
+      <c r="A13" s="10"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="11"/>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
+      <c r="A14" s="10"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="11"/>
-      <c r="B15" s="11"/>
-      <c r="C15" s="11"/>
+      <c r="A15" s="10"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="11"/>
-      <c r="B16" s="11"/>
-      <c r="C16" s="11"/>
+      <c r="A16" s="10"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="11"/>
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
+      <c r="A17" s="10"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="11"/>
-      <c r="B18" s="11"/>
-      <c r="C18" s="11"/>
+      <c r="A18" s="10"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="11"/>
-      <c r="B19" s="11"/>
-      <c r="C19" s="11"/>
+      <c r="A19" s="10"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="11"/>
-      <c r="B20" s="11"/>
-      <c r="C20" s="11"/>
+      <c r="A20" s="10"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="10"/>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="11"/>
-      <c r="B21" s="11"/>
-      <c r="C21" s="11"/>
+      <c r="A21" s="10"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="11"/>
-      <c r="B22" s="11"/>
-      <c r="C22" s="11"/>
+      <c r="A22" s="10"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="11"/>
-      <c r="B23" s="11"/>
-      <c r="C23" s="11"/>
+      <c r="A23" s="10"/>
+      <c r="B23" s="10"/>
+      <c r="C23" s="10"/>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="11"/>
-      <c r="B24" s="11"/>
-      <c r="C24" s="11"/>
+      <c r="A24" s="10"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="10"/>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="11"/>
-      <c r="B25" s="11"/>
-      <c r="C25" s="11"/>
+      <c r="A25" s="10"/>
+      <c r="B25" s="10"/>
+      <c r="C25" s="10"/>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="11"/>
-      <c r="B26" s="11"/>
-      <c r="C26" s="11"/>
+      <c r="A26" s="10"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="10"/>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="11"/>
-      <c r="B27" s="11"/>
-      <c r="C27" s="11"/>
+      <c r="A27" s="10"/>
+      <c r="B27" s="10"/>
+      <c r="C27" s="10"/>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="11"/>
-      <c r="B28" s="11"/>
-      <c r="C28" s="11"/>
+      <c r="A28" s="10"/>
+      <c r="B28" s="10"/>
+      <c r="C28" s="10"/>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="11"/>
-      <c r="B29" s="11"/>
-      <c r="C29" s="11"/>
+      <c r="A29" s="10"/>
+      <c r="B29" s="10"/>
+      <c r="C29" s="10"/>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="11"/>
-      <c r="B30" s="11"/>
-      <c r="C30" s="11"/>
+      <c r="A30" s="10"/>
+      <c r="B30" s="10"/>
+      <c r="C30" s="10"/>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="11"/>
-      <c r="B31" s="11"/>
-      <c r="C31" s="11"/>
+      <c r="A31" s="10"/>
+      <c r="B31" s="10"/>
+      <c r="C31" s="10"/>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="11"/>
-      <c r="B32" s="11"/>
-      <c r="C32" s="11"/>
+      <c r="A32" s="10"/>
+      <c r="B32" s="10"/>
+      <c r="C32" s="10"/>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="11"/>
-      <c r="B33" s="11"/>
-      <c r="C33" s="11"/>
+      <c r="A33" s="10"/>
+      <c r="B33" s="10"/>
+      <c r="C33" s="10"/>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="11"/>
-      <c r="B34" s="11"/>
-      <c r="C34" s="11"/>
+      <c r="A34" s="10"/>
+      <c r="B34" s="10"/>
+      <c r="C34" s="10"/>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="11"/>
-      <c r="B35" s="11"/>
-      <c r="C35" s="11"/>
+      <c r="A35" s="10"/>
+      <c r="B35" s="10"/>
+      <c r="C35" s="10"/>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="11"/>
-      <c r="B36" s="11"/>
-      <c r="C36" s="11"/>
+      <c r="A36" s="10"/>
+      <c r="B36" s="10"/>
+      <c r="C36" s="10"/>
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="11"/>
-      <c r="B37" s="11"/>
-      <c r="C37" s="11"/>
+      <c r="A37" s="10"/>
+      <c r="B37" s="10"/>
+      <c r="C37" s="10"/>
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="11"/>
-      <c r="B38" s="11"/>
-      <c r="C38" s="11"/>
+      <c r="A38" s="10"/>
+      <c r="B38" s="10"/>
+      <c r="C38" s="10"/>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="11"/>
-      <c r="B39" s="11"/>
-      <c r="C39" s="11"/>
+      <c r="A39" s="10"/>
+      <c r="B39" s="10"/>
+      <c r="C39" s="10"/>
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="11"/>
-      <c r="B40" s="11"/>
-      <c r="C40" s="11"/>
+      <c r="A40" s="10"/>
+      <c r="B40" s="10"/>
+      <c r="C40" s="10"/>
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="11"/>
-      <c r="B41" s="11"/>
-      <c r="C41" s="11"/>
+      <c r="A41" s="10"/>
+      <c r="B41" s="10"/>
+      <c r="C41" s="10"/>
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="11"/>
-      <c r="B42" s="11"/>
-      <c r="C42" s="11"/>
+      <c r="A42" s="10"/>
+      <c r="B42" s="10"/>
+      <c r="C42" s="10"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
feat: revoke consent clients page - create query to revoke consent clients - create revoke consent query service - create endpoint in controller to revoke consent - att documentation
</commit_message>
<xml_diff>
--- a/src/main/resources/docs/especialista-spring-rest.xlsx
+++ b/src/main/resources/docs/especialista-spring-rest.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1266" uniqueCount="1166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1269" uniqueCount="1169">
   <si>
     <t xml:space="preserve">Especialista Spring Rest</t>
   </si>
@@ -5584,6 +5584,20 @@
   </si>
   <si>
     <t xml:space="preserve">27.20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Revogando 
+Consentimentos e autorizações</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Criar query para listar as autorizações de um cliente especifico
+- Adicionar uma nova busca na interface de consent clients
+- Implementar esse novo metodo no Service
+- Ajustar o bean no authorizationServcerConfig
+- Criar um post no Controller para o revoke</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27.21</t>
   </si>
   <si>
     <t xml:space="preserve">ERRO</t>
@@ -5949,8 +5963,8 @@
   </sheetPr>
   <dimension ref="A1:F425"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A419" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B421" activeCellId="0" sqref="B421"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A417" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B423" activeCellId="0" sqref="B423"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10587,10 +10601,16 @@
         <v>1160</v>
       </c>
     </row>
-    <row r="422" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A422" s="6"/>
-      <c r="B422" s="6"/>
-      <c r="C422" s="8"/>
+    <row r="422" customFormat="false" ht="66.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A422" s="6" t="s">
+        <v>1161</v>
+      </c>
+      <c r="B422" s="6" t="s">
+        <v>1162</v>
+      </c>
+      <c r="C422" s="8" t="s">
+        <v>1163</v>
+      </c>
     </row>
     <row r="423" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A423" s="6"/>
@@ -10643,7 +10663,7 @@
   <sheetData>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>1161</v>
+        <v>1164</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>2</v>
@@ -10655,10 +10675,10 @@
         <v>400</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>1162</v>
+        <v>1165</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>1163</v>
+        <v>1166</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10666,10 +10686,10 @@
         <v>404</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>1164</v>
+        <v>1167</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>1165</v>
+        <v>1168</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
feat: update to spring 3 - remove squigly and others dependencies - update some dependencies - adjust jakarta EE and jakarta persistence 3.0 - update spring doc - update authorization server
</commit_message>
<xml_diff>
--- a/src/main/resources/docs/especialista-spring-rest.xlsx
+++ b/src/main/resources/docs/especialista-spring-rest.xlsx
@@ -5732,7 +5732,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -5765,8 +5765,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -5961,10 +5965,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F425"/>
+  <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A417" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B423" activeCellId="0" sqref="B423"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A420" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F424" activeCellId="0" sqref="F424"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10597,7 +10601,7 @@
       <c r="B421" s="6" t="s">
         <v>1159</v>
       </c>
-      <c r="C421" s="8" t="s">
+      <c r="C421" s="6" t="s">
         <v>1160</v>
       </c>
     </row>
@@ -10608,25 +10612,55 @@
       <c r="B422" s="6" t="s">
         <v>1162</v>
       </c>
-      <c r="C422" s="8" t="s">
+      <c r="C422" s="6" t="s">
         <v>1163</v>
       </c>
     </row>
     <row r="423" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A423" s="6"/>
       <c r="B423" s="6"/>
-      <c r="C423" s="8"/>
+      <c r="C423" s="6"/>
     </row>
     <row r="424" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A424" s="6"/>
       <c r="B424" s="6"/>
-      <c r="C424" s="8"/>
+      <c r="C424" s="6"/>
     </row>
     <row r="425" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A425" s="6"/>
       <c r="B425" s="6"/>
-      <c r="C425" s="8"/>
-    </row>
+      <c r="C425" s="6"/>
+    </row>
+    <row r="426" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A426" s="8"/>
+      <c r="B426" s="8"/>
+      <c r="C426" s="9"/>
+    </row>
+    <row r="427" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A427" s="8"/>
+      <c r="B427" s="8"/>
+      <c r="C427" s="9"/>
+    </row>
+    <row r="428" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A428" s="8"/>
+      <c r="B428" s="8"/>
+      <c r="C428" s="9"/>
+    </row>
+    <row r="429" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A429" s="8"/>
+      <c r="B429" s="8"/>
+      <c r="C429" s="9"/>
+    </row>
+    <row r="430" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A430" s="8"/>
+      <c r="B430" s="8"/>
+      <c r="C430" s="9"/>
+    </row>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:C1"/>
@@ -10662,225 +10696,225 @@
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="10" t="s">
         <v>1164</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="10"/>
+      <c r="C2" s="11"/>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="10" t="n">
+      <c r="A3" s="11" t="n">
         <v>400</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="11" t="s">
         <v>1165</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="11" t="s">
         <v>1166</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="10" t="n">
+      <c r="A4" s="11" t="n">
         <v>404</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="11" t="s">
         <v>1167</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="11" t="s">
         <v>1168</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="10"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
+      <c r="A5" s="11"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="10"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
+      <c r="A6" s="11"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="10"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
+      <c r="A7" s="11"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="10"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
+      <c r="A8" s="11"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="10"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
+      <c r="A9" s="11"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="10"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
+      <c r="A10" s="11"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="10"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
+      <c r="A11" s="11"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="10"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
+      <c r="A12" s="11"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="10"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
+      <c r="A13" s="11"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="10"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
+      <c r="A14" s="11"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="10"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
+      <c r="A15" s="11"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="10"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="10"/>
+      <c r="A16" s="11"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="10"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
+      <c r="A17" s="11"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="10"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="10"/>
+      <c r="A18" s="11"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="10"/>
-      <c r="B19" s="10"/>
-      <c r="C19" s="10"/>
+      <c r="A19" s="11"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="10"/>
-      <c r="B20" s="10"/>
-      <c r="C20" s="10"/>
+      <c r="A20" s="11"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="11"/>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="10"/>
-      <c r="B21" s="10"/>
-      <c r="C21" s="10"/>
+      <c r="A21" s="11"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="11"/>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="10"/>
-      <c r="B22" s="10"/>
-      <c r="C22" s="10"/>
+      <c r="A22" s="11"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="11"/>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="10"/>
-      <c r="B23" s="10"/>
-      <c r="C23" s="10"/>
+      <c r="A23" s="11"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="11"/>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="10"/>
-      <c r="B24" s="10"/>
-      <c r="C24" s="10"/>
+      <c r="A24" s="11"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="11"/>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="10"/>
-      <c r="B25" s="10"/>
-      <c r="C25" s="10"/>
+      <c r="A25" s="11"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="10"/>
-      <c r="B26" s="10"/>
-      <c r="C26" s="10"/>
+      <c r="A26" s="11"/>
+      <c r="B26" s="11"/>
+      <c r="C26" s="11"/>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="10"/>
-      <c r="B27" s="10"/>
-      <c r="C27" s="10"/>
+      <c r="A27" s="11"/>
+      <c r="B27" s="11"/>
+      <c r="C27" s="11"/>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="10"/>
-      <c r="B28" s="10"/>
-      <c r="C28" s="10"/>
+      <c r="A28" s="11"/>
+      <c r="B28" s="11"/>
+      <c r="C28" s="11"/>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="10"/>
-      <c r="B29" s="10"/>
-      <c r="C29" s="10"/>
+      <c r="A29" s="11"/>
+      <c r="B29" s="11"/>
+      <c r="C29" s="11"/>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="10"/>
-      <c r="B30" s="10"/>
-      <c r="C30" s="10"/>
+      <c r="A30" s="11"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="11"/>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="10"/>
-      <c r="B31" s="10"/>
-      <c r="C31" s="10"/>
+      <c r="A31" s="11"/>
+      <c r="B31" s="11"/>
+      <c r="C31" s="11"/>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="10"/>
-      <c r="B32" s="10"/>
-      <c r="C32" s="10"/>
+      <c r="A32" s="11"/>
+      <c r="B32" s="11"/>
+      <c r="C32" s="11"/>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="10"/>
-      <c r="B33" s="10"/>
-      <c r="C33" s="10"/>
+      <c r="A33" s="11"/>
+      <c r="B33" s="11"/>
+      <c r="C33" s="11"/>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="10"/>
-      <c r="B34" s="10"/>
-      <c r="C34" s="10"/>
+      <c r="A34" s="11"/>
+      <c r="B34" s="11"/>
+      <c r="C34" s="11"/>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="10"/>
-      <c r="B35" s="10"/>
-      <c r="C35" s="10"/>
+      <c r="A35" s="11"/>
+      <c r="B35" s="11"/>
+      <c r="C35" s="11"/>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="10"/>
-      <c r="B36" s="10"/>
-      <c r="C36" s="10"/>
+      <c r="A36" s="11"/>
+      <c r="B36" s="11"/>
+      <c r="C36" s="11"/>
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="10"/>
-      <c r="B37" s="10"/>
-      <c r="C37" s="10"/>
+      <c r="A37" s="11"/>
+      <c r="B37" s="11"/>
+      <c r="C37" s="11"/>
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="10"/>
-      <c r="B38" s="10"/>
-      <c r="C38" s="10"/>
+      <c r="A38" s="11"/>
+      <c r="B38" s="11"/>
+      <c r="C38" s="11"/>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="10"/>
-      <c r="B39" s="10"/>
-      <c r="C39" s="10"/>
+      <c r="A39" s="11"/>
+      <c r="B39" s="11"/>
+      <c r="C39" s="11"/>
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="10"/>
-      <c r="B40" s="10"/>
-      <c r="C40" s="10"/>
+      <c r="A40" s="11"/>
+      <c r="B40" s="11"/>
+      <c r="C40" s="11"/>
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="10"/>
-      <c r="B41" s="10"/>
-      <c r="C41" s="10"/>
+      <c r="A41" s="11"/>
+      <c r="B41" s="11"/>
+      <c r="C41" s="11"/>
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="10"/>
-      <c r="B42" s="10"/>
-      <c r="C42" s="10"/>
+      <c r="A42" s="11"/>
+      <c r="B42" s="11"/>
+      <c r="C42" s="11"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>